<commit_message>
copied over target files from DR5_target_updates branch on old ullyse_tech repo to new repo ullyses-utils
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F45E47-7C79-8340-ADCE-9011424652A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A83CC5A-8213-9840-B097-7141E00C59EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="920" windowWidth="35780" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="460" windowWidth="34740" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -2094,7 +2094,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
@@ -2104,6 +2104,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3172,9 +3174,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V53" sqref="V53"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A26" sqref="A26"/>
+      <selection pane="topRight" activeCell="A15" sqref="A15:X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5556,76 +5559,80 @@
       <c r="X31" s="7"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="9">
         <v>200</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="9">
         <v>0.44</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="9">
         <v>-8.76</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="9">
         <v>0.8</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="9">
         <v>13.89</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="9">
         <v>13.44</v>
       </c>
-      <c r="N32">
-        <v>1</v>
-      </c>
-      <c r="O32">
+      <c r="N32" s="9">
+        <v>1</v>
+      </c>
+      <c r="O32" s="9">
         <v>7</v>
       </c>
-      <c r="P32">
-        <v>1</v>
-      </c>
-      <c r="Q32">
+      <c r="P32" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="9">
         <v>10.37</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="9">
         <v>0.43</v>
       </c>
-      <c r="T32">
+      <c r="T32" s="9">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="U32">
+      <c r="U32" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V32">
+      <c r="V32" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
+      <c r="W32" s="10">
+        <v>16855</v>
+      </c>
+      <c r="X32" s="9"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -7027,793 +7034,838 @@
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="A52" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="9">
         <v>200</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="9">
         <v>0.22</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="9">
         <v>-8.5299999999999994</v>
       </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52">
+      <c r="K52" s="9">
+        <v>0</v>
+      </c>
+      <c r="L52" s="9">
         <v>14.51</v>
       </c>
-      <c r="M52">
+      <c r="M52" s="9">
         <v>14.58</v>
       </c>
-      <c r="N52">
-        <v>1</v>
-      </c>
-      <c r="O52">
-        <v>1</v>
-      </c>
-      <c r="P52">
-        <v>1</v>
-      </c>
-      <c r="Q52">
+      <c r="N52" s="9">
+        <v>1</v>
+      </c>
+      <c r="O52" s="9">
+        <v>1</v>
+      </c>
+      <c r="P52" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R52">
+      <c r="R52" s="9">
         <v>1.28</v>
       </c>
-      <c r="S52">
+      <c r="S52" s="9">
         <v>0.23</v>
       </c>
-      <c r="T52">
+      <c r="T52" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U52">
+      <c r="U52" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V52">
+      <c r="V52" s="9">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
+      <c r="W52" s="9">
+        <v>16856</v>
+      </c>
+      <c r="X52" s="9"/>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="A53" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="9">
         <v>130</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="9">
         <v>0.93</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="9">
         <v>-8.8000000000000007</v>
       </c>
-      <c r="K53">
+      <c r="K53" s="9">
         <v>0.4</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="9">
         <v>12.06</v>
       </c>
-      <c r="M53">
+      <c r="M53" s="9">
         <v>11.77</v>
       </c>
-      <c r="N53">
-        <v>1</v>
-      </c>
-      <c r="O53">
+      <c r="N53" s="9">
+        <v>1</v>
+      </c>
+      <c r="O53" s="9">
         <v>2</v>
       </c>
-      <c r="P53">
-        <v>1</v>
-      </c>
-      <c r="Q53">
+      <c r="P53" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R53">
+      <c r="R53" s="9">
         <v>2.04</v>
       </c>
-      <c r="S53">
+      <c r="S53" s="9">
         <v>0.24</v>
       </c>
-      <c r="T53">
+      <c r="T53" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U53">
+      <c r="U53" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V53">
+      <c r="V53" s="9">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
+      <c r="W53" s="10">
+        <v>16859</v>
+      </c>
+      <c r="X53" s="9"/>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="A54" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="D54" t="s">
+      <c r="C54" s="9"/>
+      <c r="D54" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="9">
         <v>150</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="I54">
+      <c r="I54" s="9">
         <v>0.16</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="9">
         <v>-9.2100000000000009</v>
       </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-      <c r="L54">
+      <c r="K54" s="9">
+        <v>0</v>
+      </c>
+      <c r="L54" s="9">
         <v>16.510000000000002</v>
       </c>
-      <c r="M54">
+      <c r="M54" s="9">
         <v>16.16</v>
       </c>
-      <c r="N54">
-        <v>1</v>
-      </c>
-      <c r="O54">
+      <c r="N54" s="9">
+        <v>1</v>
+      </c>
+      <c r="O54" s="9">
         <v>2</v>
       </c>
-      <c r="P54">
-        <v>1</v>
-      </c>
-      <c r="Q54">
+      <c r="P54" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R54">
+      <c r="R54" s="9">
         <v>2.09</v>
       </c>
-      <c r="S54">
+      <c r="S54" s="9">
         <v>0.26</v>
       </c>
-      <c r="T54">
+      <c r="T54" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U54">
+      <c r="U54" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V54">
+      <c r="V54" s="9">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
+      <c r="W54" s="9">
+        <v>16853</v>
+      </c>
+      <c r="X54" s="9"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="A55" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="9">
         <v>150</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="9">
         <v>0.5</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="9">
         <v>-7.92</v>
       </c>
-      <c r="K55">
-        <v>1</v>
-      </c>
-      <c r="L55">
+      <c r="K55" s="9">
+        <v>1</v>
+      </c>
+      <c r="L55" s="9">
         <v>14.91</v>
       </c>
-      <c r="M55">
+      <c r="M55" s="9">
         <v>13.85</v>
       </c>
-      <c r="N55">
-        <v>1</v>
-      </c>
-      <c r="O55">
+      <c r="N55" s="9">
+        <v>1</v>
+      </c>
+      <c r="O55" s="9">
         <v>3</v>
       </c>
-      <c r="P55">
-        <v>1</v>
-      </c>
-      <c r="Q55">
+      <c r="P55" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R55">
+      <c r="R55" s="9">
         <v>5.25</v>
       </c>
-      <c r="S55">
+      <c r="S55" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T55">
+      <c r="T55" s="9">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="U55">
+      <c r="U55" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V55">
+      <c r="V55" s="9">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
+      <c r="W55" s="9">
+        <v>16853</v>
+      </c>
+      <c r="X55" s="9"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="A56" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="9">
         <v>150</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="9">
         <v>0.95</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="9">
         <v>-8.0399999999999991</v>
       </c>
-      <c r="K56">
+      <c r="K56" s="9">
         <v>0.9</v>
       </c>
-      <c r="L56">
+      <c r="L56" s="9">
         <v>11.99</v>
       </c>
-      <c r="M56">
+      <c r="M56" s="9">
         <v>11.93</v>
       </c>
-      <c r="N56">
-        <v>1</v>
-      </c>
-      <c r="O56">
+      <c r="N56" s="9">
+        <v>1</v>
+      </c>
+      <c r="O56" s="9">
         <v>3</v>
       </c>
-      <c r="P56">
-        <v>1</v>
-      </c>
-      <c r="Q56">
+      <c r="P56" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R56">
+      <c r="R56" s="9">
         <v>5.07</v>
       </c>
-      <c r="S56">
+      <c r="S56" s="9">
         <v>0.3</v>
       </c>
-      <c r="T56">
+      <c r="T56" s="9">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U56">
+      <c r="U56" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V56">
+      <c r="V56" s="9">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="W56" s="9">
+        <v>16853</v>
+      </c>
+      <c r="X56" s="9"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="9">
         <v>200</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="9">
         <v>0.21</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="9">
         <v>-8.9600000000000009</v>
       </c>
-      <c r="K57">
+      <c r="K57" s="9">
         <v>0.3</v>
       </c>
-      <c r="L57">
+      <c r="L57" s="9">
         <v>14.46</v>
       </c>
-      <c r="M57">
+      <c r="M57" s="9">
         <v>14.12</v>
       </c>
-      <c r="N57">
-        <v>1</v>
-      </c>
-      <c r="O57">
+      <c r="N57" s="9">
+        <v>1</v>
+      </c>
+      <c r="O57" s="9">
         <v>3</v>
       </c>
-      <c r="P57">
-        <v>1</v>
-      </c>
-      <c r="Q57">
+      <c r="P57" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R57">
+      <c r="R57" s="9">
         <v>4.3499999999999996</v>
       </c>
-      <c r="S57">
+      <c r="S57" s="9">
         <v>0.33</v>
       </c>
-      <c r="T57">
+      <c r="T57" s="9">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U57">
+      <c r="U57" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V57">
+      <c r="V57" s="9">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="W57" s="9">
+        <v>16857</v>
+      </c>
+      <c r="X57" s="9"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="9">
         <v>200</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="9">
         <v>0.23</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="9">
         <v>-9.41</v>
       </c>
-      <c r="K58">
-        <v>0</v>
-      </c>
-      <c r="L58">
+      <c r="K58" s="9">
+        <v>0</v>
+      </c>
+      <c r="L58" s="9">
         <v>16.47</v>
       </c>
-      <c r="M58">
+      <c r="M58" s="9">
         <v>16</v>
       </c>
-      <c r="N58">
-        <v>1</v>
-      </c>
-      <c r="O58">
+      <c r="N58" s="9">
+        <v>1</v>
+      </c>
+      <c r="O58" s="9">
         <v>3</v>
       </c>
-      <c r="P58">
-        <v>1</v>
-      </c>
-      <c r="Q58">
+      <c r="P58" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q58" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R58">
+      <c r="R58" s="9">
         <v>4.67</v>
       </c>
-      <c r="S58">
+      <c r="S58" s="9">
         <v>0.37</v>
       </c>
-      <c r="T58">
+      <c r="T58" s="9">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U58">
+      <c r="U58" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V58">
+      <c r="V58" s="9">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="W58" s="9">
+        <v>16856</v>
+      </c>
+      <c r="X58" s="9"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="A59" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="9">
         <v>200</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="9">
         <v>0.26</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="9">
         <v>-8.61</v>
       </c>
-      <c r="K59">
+      <c r="K59" s="9">
         <v>0.5</v>
       </c>
-      <c r="L59">
+      <c r="L59" s="9">
         <v>14.81</v>
       </c>
-      <c r="M59">
+      <c r="M59" s="9">
         <v>14.59</v>
       </c>
-      <c r="N59">
-        <v>1</v>
-      </c>
-      <c r="O59">
+      <c r="N59" s="9">
+        <v>1</v>
+      </c>
+      <c r="O59" s="9">
         <v>3</v>
       </c>
-      <c r="P59">
-        <v>1</v>
-      </c>
-      <c r="Q59">
+      <c r="P59" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R59">
+      <c r="R59" s="9">
         <v>3.82</v>
       </c>
-      <c r="S59">
+      <c r="S59" s="9">
         <v>0.3</v>
       </c>
-      <c r="T59">
+      <c r="T59" s="9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U59">
+      <c r="U59" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V59">
+      <c r="V59" s="9">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
+      <c r="W59" s="9">
+        <v>16855</v>
+      </c>
+      <c r="X59" s="9"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="A60" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="9">
         <v>200</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="9">
         <v>0.23</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="9">
         <v>-9.5299999999999994</v>
       </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
+      <c r="K60" s="9">
+        <v>0</v>
+      </c>
+      <c r="L60" s="9">
         <v>15.15</v>
       </c>
-      <c r="M60">
+      <c r="M60" s="9">
         <v>14.61</v>
       </c>
-      <c r="N60">
-        <v>1</v>
-      </c>
-      <c r="O60">
+      <c r="N60" s="9">
+        <v>1</v>
+      </c>
+      <c r="O60" s="9">
         <v>4</v>
       </c>
-      <c r="P60">
-        <v>1</v>
-      </c>
-      <c r="Q60">
+      <c r="P60" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R60">
+      <c r="R60" s="9">
         <v>5.75</v>
       </c>
-      <c r="S60">
+      <c r="S60" s="9">
         <v>0.41</v>
       </c>
-      <c r="T60">
+      <c r="T60" s="9">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="U60">
+      <c r="U60" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V60">
+      <c r="V60" s="9">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
+      <c r="W60" s="9">
+        <v>16855</v>
+      </c>
+      <c r="X60" s="9"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="9">
         <v>200</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="9">
         <v>0.16</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="9">
         <v>-9.44</v>
       </c>
-      <c r="K61">
-        <v>0</v>
-      </c>
-      <c r="L61">
+      <c r="K61" s="9">
+        <v>0</v>
+      </c>
+      <c r="L61" s="9">
         <v>15.92</v>
       </c>
-      <c r="M61">
+      <c r="M61" s="9">
         <v>15.43</v>
       </c>
-      <c r="N61">
-        <v>1</v>
-      </c>
-      <c r="O61">
+      <c r="N61" s="9">
+        <v>1</v>
+      </c>
+      <c r="O61" s="9">
         <v>4</v>
       </c>
-      <c r="P61">
-        <v>1</v>
-      </c>
-      <c r="Q61">
+      <c r="P61" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R61">
+      <c r="R61" s="9">
         <v>4.91</v>
       </c>
-      <c r="S61">
+      <c r="S61" s="9">
         <v>0.38</v>
       </c>
-      <c r="T61">
+      <c r="T61" s="9">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U61">
+      <c r="U61" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V61">
+      <c r="V61" s="9">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="W61" s="9">
+        <v>16858</v>
+      </c>
+      <c r="X61" s="9"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="9">
         <v>200</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="9">
         <v>0.7</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="9">
         <v>-7.23</v>
       </c>
-      <c r="K62">
-        <v>1</v>
-      </c>
-      <c r="L62">
+      <c r="K62" s="9">
+        <v>1</v>
+      </c>
+      <c r="L62" s="9">
         <v>13.27</v>
       </c>
-      <c r="M62">
+      <c r="M62" s="9">
         <v>13.66</v>
       </c>
-      <c r="N62">
-        <v>1</v>
-      </c>
-      <c r="O62">
+      <c r="N62" s="9">
+        <v>1</v>
+      </c>
+      <c r="O62" s="9">
         <v>5</v>
       </c>
-      <c r="P62">
-        <v>1</v>
-      </c>
-      <c r="Q62">
+      <c r="P62" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="R62">
+      <c r="R62" s="9">
         <v>8.86</v>
       </c>
-      <c r="S62">
+      <c r="S62" s="9">
         <v>0.22</v>
       </c>
-      <c r="T62">
+      <c r="T62" s="9">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="U62">
+      <c r="U62" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V62">
+      <c r="V62" s="9">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
+      <c r="W62" s="9">
+        <v>16854</v>
+      </c>
+      <c r="X62" s="9"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
@@ -7888,361 +7940,380 @@
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="A64" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="D64" t="s">
+      <c r="C64" s="9"/>
+      <c r="D64" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="9">
         <v>130</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="I64">
+      <c r="I64" s="9">
         <v>1.04</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="9">
         <v>-8.6999999999999993</v>
       </c>
-      <c r="K64">
-        <v>1</v>
-      </c>
-      <c r="L64">
+      <c r="K64" s="9">
+        <v>1</v>
+      </c>
+      <c r="L64" s="9">
         <v>12.7</v>
       </c>
-      <c r="M64">
+      <c r="M64" s="9">
         <v>12.19</v>
       </c>
-      <c r="N64">
-        <v>1</v>
-      </c>
-      <c r="O64">
+      <c r="N64" s="9">
+        <v>1</v>
+      </c>
+      <c r="O64" s="9">
         <v>6</v>
       </c>
-      <c r="P64">
-        <v>1</v>
-      </c>
-      <c r="Q64">
+      <c r="P64" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R64">
+      <c r="R64" s="9">
         <v>6.79</v>
       </c>
-      <c r="S64">
+      <c r="S64" s="9">
         <v>0.31</v>
       </c>
-      <c r="T64">
+      <c r="T64" s="9">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="U64">
+      <c r="U64" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V64">
+      <c r="V64" s="9">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
+      <c r="W64" s="9">
+        <v>16859</v>
+      </c>
+      <c r="X64" s="9"/>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="A65" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="9">
         <v>150</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I65">
+      <c r="I65" s="9">
         <v>0.79</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="9">
         <v>-8.4</v>
       </c>
-      <c r="K65">
+      <c r="K65" s="9">
         <v>0.9</v>
       </c>
-      <c r="L65">
+      <c r="L65" s="9">
         <v>12.28</v>
       </c>
-      <c r="M65">
+      <c r="M65" s="9">
         <v>12</v>
       </c>
-      <c r="N65">
-        <v>1</v>
-      </c>
-      <c r="O65">
+      <c r="N65" s="9">
+        <v>1</v>
+      </c>
+      <c r="O65" s="9">
         <v>6</v>
       </c>
-      <c r="P65">
-        <v>1</v>
-      </c>
-      <c r="Q65">
+      <c r="P65" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R65">
+      <c r="R65" s="9">
         <v>10.52</v>
       </c>
-      <c r="S65">
+      <c r="S65" s="9">
         <v>0.39</v>
       </c>
-      <c r="T65">
+      <c r="T65" s="9">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="U65">
+      <c r="U65" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V65">
+      <c r="V65" s="9">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
+      <c r="W65" s="9">
+        <v>16854</v>
+      </c>
+      <c r="X65" s="9"/>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="9">
         <v>200</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="I66">
+      <c r="I66" s="9">
         <v>0.16</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="9">
         <v>-9.75</v>
       </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66">
+      <c r="K66" s="9">
+        <v>0</v>
+      </c>
+      <c r="L66" s="9">
         <v>15.93</v>
       </c>
-      <c r="M66">
+      <c r="M66" s="9">
         <v>15.25</v>
       </c>
-      <c r="N66">
-        <v>1</v>
-      </c>
-      <c r="O66">
+      <c r="N66" s="9">
+        <v>1</v>
+      </c>
+      <c r="O66" s="9">
         <v>6</v>
       </c>
-      <c r="P66">
-        <v>1</v>
-      </c>
-      <c r="Q66">
+      <c r="P66" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R66">
+      <c r="R66" s="9">
         <v>8.5500000000000007</v>
       </c>
-      <c r="S66">
+      <c r="S66" s="9">
         <v>0.5</v>
       </c>
-      <c r="T66">
+      <c r="T66" s="9">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="U66">
+      <c r="U66" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V66">
+      <c r="V66" s="9">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
+      <c r="W66" s="9">
+        <v>16858</v>
+      </c>
+      <c r="X66" s="9"/>
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="A67" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="9" t="s">
         <v>344</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="9">
         <v>200</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="I67">
+      <c r="I67" s="9">
         <v>0.22</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="9">
         <v>-8.99</v>
       </c>
-      <c r="K67">
+      <c r="K67" s="9">
         <v>0.7</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="9">
         <v>11.69</v>
       </c>
-      <c r="M67">
+      <c r="M67" s="9">
         <v>11.14</v>
       </c>
-      <c r="N67">
-        <v>1</v>
-      </c>
-      <c r="O67">
+      <c r="N67" s="9">
+        <v>1</v>
+      </c>
+      <c r="O67" s="9">
         <v>8</v>
       </c>
-      <c r="P67">
-        <v>1</v>
-      </c>
-      <c r="Q67">
+      <c r="P67" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="9">
         <f t="shared" ref="Q67:Q69" si="7">O67+P67</f>
         <v>9</v>
       </c>
-      <c r="R67">
+      <c r="R67" s="9">
         <v>12.36</v>
       </c>
-      <c r="S67">
+      <c r="S67" s="9">
         <v>0.48</v>
       </c>
-      <c r="T67">
+      <c r="T67" s="9">
         <f t="shared" ref="T67:T68" si="8">ROUND(R67+0.3,0)</f>
         <v>13</v>
       </c>
-      <c r="U67">
+      <c r="U67" s="9">
         <f t="shared" ref="U67:U69" si="9">CEILING(S67,1)</f>
         <v>1</v>
       </c>
-      <c r="V67">
+      <c r="V67" s="9">
         <f t="shared" ref="V67:V68" si="10">(T67+U67)*N67</f>
         <v>14</v>
       </c>
+      <c r="W67" s="9">
+        <v>16856</v>
+      </c>
+      <c r="X67" s="9"/>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="A68" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="9">
         <v>200</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H68" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="9">
         <v>0.19</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="9">
         <v>-9.24</v>
       </c>
-      <c r="K68">
+      <c r="K68" s="9">
         <v>0.5</v>
       </c>
-      <c r="L68">
+      <c r="L68" s="9">
         <v>16.09</v>
       </c>
-      <c r="M68">
+      <c r="M68" s="9">
         <v>15.48</v>
       </c>
-      <c r="N68">
-        <v>1</v>
-      </c>
-      <c r="O68">
+      <c r="N68" s="9">
+        <v>1</v>
+      </c>
+      <c r="O68" s="9">
         <v>8</v>
       </c>
-      <c r="P68">
-        <v>1</v>
-      </c>
-      <c r="Q68">
+      <c r="P68" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="9">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="R68">
+      <c r="R68" s="9">
         <v>11.82</v>
       </c>
-      <c r="S68">
+      <c r="S68" s="9">
         <v>0.5</v>
       </c>
-      <c r="T68">
-        <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="U68">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="V68">
+      <c r="T68" s="9">
+        <v>0</v>
+      </c>
+      <c r="U68" s="9">
+        <v>9</v>
+      </c>
+      <c r="V68" s="9">
         <f t="shared" si="10"/>
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="W68" s="9">
+        <v>16857</v>
+      </c>
+      <c r="X68" s="9"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">

</xml_diff>

<commit_message>
added a few AR ctts_ar_data_check
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A83CC5A-8213-9840-B097-7141E00C59EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDE8856-29F2-304A-B410-8746D3E34039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="460" windowWidth="34740" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="460" windowWidth="23460" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="563">
   <si>
     <t>2MASS</t>
   </si>
@@ -1604,6 +1604,120 @@
   </si>
   <si>
     <t xml:space="preserve">Sigma Ori </t>
+  </si>
+  <si>
+    <t>FM Tau</t>
+  </si>
+  <si>
+    <t>4h14m13.56s</t>
+  </si>
+  <si>
+    <t>+28d12m48.8s</t>
+  </si>
+  <si>
+    <t>J04141358+2812492</t>
+  </si>
+  <si>
+    <t>HBC 23</t>
+  </si>
+  <si>
+    <t>COS/130M-COS/G160M-STIS/E230M-STIS/G230L-STIS/G430L</t>
+  </si>
+  <si>
+    <t>HN Tau A</t>
+  </si>
+  <si>
+    <t>4h33mm39.37s</t>
+  </si>
+  <si>
+    <t>+17d51m52.1s</t>
+  </si>
+  <si>
+    <t>8238|11616|11660</t>
+  </si>
+  <si>
+    <t>COS/130M-COS/G160M-STIS/E230M-STIS/G230L-STIS/G430L-STIS/G750L</t>
+  </si>
+  <si>
+    <t>J04333935+1751523</t>
+  </si>
+  <si>
+    <t>HBC 60</t>
+  </si>
+  <si>
+    <t>IP Tau</t>
+  </si>
+  <si>
+    <t>4h24m57.14s</t>
+  </si>
+  <si>
+    <t>+27d11m56.4s</t>
+  </si>
+  <si>
+    <t>HBC 385</t>
+  </si>
+  <si>
+    <t>J04245708+2711565</t>
+  </si>
+  <si>
+    <t>PDS 66</t>
+  </si>
+  <si>
+    <t>13h22m07.45s</t>
+  </si>
+  <si>
+    <t>-69d38m12.6s</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>J13220753-6938121</t>
+  </si>
+  <si>
+    <t>Lower Centaurus-Crux</t>
+  </si>
+  <si>
+    <t>MP MUS</t>
+  </si>
+  <si>
+    <t>STIS/E140M-STIS/E230M-STIS/G230L-STIS/G430L</t>
+  </si>
+  <si>
+    <t>STIS/E230M-STIS/G230L-STIS/G430L</t>
+  </si>
+  <si>
+    <t>bad data</t>
+  </si>
+  <si>
+    <t>RW Aur A</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>05h07m49.51s</t>
+  </si>
+  <si>
+    <t>+30d24m04.8s</t>
+  </si>
+  <si>
+    <t>8627|9435|11616</t>
+  </si>
+  <si>
+    <t>COS/130M-COS/G160M-STIS/G230L-STIS/G430L-STIS/G230M-STIS/E230M-STIS/G750M</t>
+  </si>
+  <si>
+    <t>TWA 3A</t>
+  </si>
+  <si>
+    <t>11h10m27.80s</t>
+  </si>
+  <si>
+    <t>-37d31m51.2s</t>
+  </si>
+  <si>
+    <t>STIS/G140M-STIS/G140L-STIS/E230M-STIS/G230L-STIS/G430L</t>
   </si>
 </sst>
 </file>
@@ -2094,7 +2208,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
@@ -2106,6 +2220,8 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2151,7 +2267,217 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="92">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3172,12 +3498,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y91"/>
+  <dimension ref="A1:Y97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="108" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A26" sqref="A26"/>
-      <selection pane="topRight" activeCell="A15" sqref="A15:X15"/>
+      <selection pane="topRight" activeCell="Y99" sqref="Y99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8225,7 +8551,7 @@
         <v>0.48</v>
       </c>
       <c r="T67" s="9">
-        <f t="shared" ref="T67:T68" si="8">ROUND(R67+0.3,0)</f>
+        <f t="shared" ref="T67" si="8">ROUND(R67+0.3,0)</f>
         <v>13</v>
       </c>
       <c r="U67" s="9">
@@ -10037,312 +10363,820 @@
         <v>3</v>
       </c>
     </row>
+    <row r="92" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>525</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="C92" t="s">
+        <v>529</v>
+      </c>
+      <c r="D92" t="s">
+        <v>526</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="F92" t="s">
+        <v>357</v>
+      </c>
+      <c r="G92">
+        <v>140</v>
+      </c>
+      <c r="H92" t="s">
+        <v>20</v>
+      </c>
+      <c r="I92">
+        <v>0.6</v>
+      </c>
+      <c r="J92">
+        <v>-8.92</v>
+      </c>
+      <c r="K92">
+        <v>0.7</v>
+      </c>
+      <c r="L92">
+        <v>14.44</v>
+      </c>
+      <c r="M92">
+        <v>13.8</v>
+      </c>
+      <c r="N92">
+        <v>2</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
+      <c r="R92">
+        <v>0</v>
+      </c>
+      <c r="S92">
+        <v>0</v>
+      </c>
+      <c r="T92">
+        <v>0</v>
+      </c>
+      <c r="U92">
+        <v>0</v>
+      </c>
+      <c r="V92">
+        <v>0</v>
+      </c>
+      <c r="W92">
+        <v>11616</v>
+      </c>
+      <c r="X92" t="s">
+        <v>551</v>
+      </c>
+      <c r="Y92" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>531</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="C93" t="s">
+        <v>537</v>
+      </c>
+      <c r="D93" t="s">
+        <v>532</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="F93" t="s">
+        <v>357</v>
+      </c>
+      <c r="G93">
+        <v>140</v>
+      </c>
+      <c r="H93" t="s">
+        <v>290</v>
+      </c>
+      <c r="I93">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J93">
+        <v>-7.85</v>
+      </c>
+      <c r="K93">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M93">
+        <v>13.4</v>
+      </c>
+      <c r="N93">
+        <v>2</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="Q93">
+        <v>0</v>
+      </c>
+      <c r="R93">
+        <v>0</v>
+      </c>
+      <c r="S93">
+        <v>0</v>
+      </c>
+      <c r="T93">
+        <v>0</v>
+      </c>
+      <c r="U93">
+        <v>0</v>
+      </c>
+      <c r="V93">
+        <v>0</v>
+      </c>
+      <c r="W93" t="s">
+        <v>534</v>
+      </c>
+      <c r="X93" t="s">
+        <v>535</v>
+      </c>
+      <c r="Y93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>538</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="C94" t="s">
+        <v>541</v>
+      </c>
+      <c r="D94" t="s">
+        <v>539</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="F94" t="s">
+        <v>357</v>
+      </c>
+      <c r="G94">
+        <v>140</v>
+      </c>
+      <c r="H94" t="s">
+        <v>20</v>
+      </c>
+      <c r="I94">
+        <v>0.6</v>
+      </c>
+      <c r="J94">
+        <v>-8.14</v>
+      </c>
+      <c r="K94">
+        <v>1.7</v>
+      </c>
+      <c r="N94">
+        <v>2</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="Q94">
+        <v>0</v>
+      </c>
+      <c r="R94">
+        <v>0</v>
+      </c>
+      <c r="S94">
+        <v>0</v>
+      </c>
+      <c r="T94">
+        <v>0</v>
+      </c>
+      <c r="U94">
+        <v>0</v>
+      </c>
+      <c r="V94">
+        <v>0</v>
+      </c>
+      <c r="W94">
+        <v>11616</v>
+      </c>
+      <c r="X94" t="s">
+        <v>530</v>
+      </c>
+      <c r="Y94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>549</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="C95" t="s">
+        <v>543</v>
+      </c>
+      <c r="D95" t="s">
+        <v>544</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="F95" t="s">
+        <v>548</v>
+      </c>
+      <c r="G95">
+        <v>86</v>
+      </c>
+      <c r="H95" t="s">
+        <v>546</v>
+      </c>
+      <c r="I95">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J95">
+        <v>-9.89</v>
+      </c>
+      <c r="K95">
+        <v>0.2</v>
+      </c>
+      <c r="M95">
+        <v>10.39</v>
+      </c>
+      <c r="N95">
+        <v>2</v>
+      </c>
+      <c r="O95">
+        <v>0</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
+      <c r="R95">
+        <v>0</v>
+      </c>
+      <c r="S95">
+        <v>0</v>
+      </c>
+      <c r="T95">
+        <v>0</v>
+      </c>
+      <c r="U95">
+        <v>0</v>
+      </c>
+      <c r="V95">
+        <v>0</v>
+      </c>
+      <c r="W95">
+        <v>11616</v>
+      </c>
+      <c r="X95" t="s">
+        <v>550</v>
+      </c>
+      <c r="Y95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>553</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="D96" s="12" t="s">
+        <v>555</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G96">
+        <v>140</v>
+      </c>
+      <c r="H96" t="s">
+        <v>554</v>
+      </c>
+      <c r="I96">
+        <v>0.9</v>
+      </c>
+      <c r="J96">
+        <v>-7.7</v>
+      </c>
+      <c r="K96">
+        <v>0.5</v>
+      </c>
+      <c r="N96">
+        <v>2</v>
+      </c>
+      <c r="O96">
+        <v>0</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="R96">
+        <v>0</v>
+      </c>
+      <c r="S96">
+        <v>0</v>
+      </c>
+      <c r="T96">
+        <v>0</v>
+      </c>
+      <c r="U96">
+        <v>0</v>
+      </c>
+      <c r="V96">
+        <v>0</v>
+      </c>
+      <c r="W96" t="s">
+        <v>557</v>
+      </c>
+      <c r="X96" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>559</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="E97" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="F97" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G97">
+        <v>56</v>
+      </c>
+      <c r="H97" t="s">
+        <v>51</v>
+      </c>
+      <c r="I97">
+        <v>0.3</v>
+      </c>
+      <c r="J97">
+        <v>-10.01</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>12.57</v>
+      </c>
+      <c r="N97">
+        <v>2</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="Q97">
+        <v>0</v>
+      </c>
+      <c r="R97">
+        <v>0</v>
+      </c>
+      <c r="S97">
+        <v>0</v>
+      </c>
+      <c r="T97">
+        <v>0</v>
+      </c>
+      <c r="U97">
+        <v>0</v>
+      </c>
+      <c r="V97">
+        <v>0</v>
+      </c>
+      <c r="W97">
+        <v>11616</v>
+      </c>
+      <c r="X97" t="s">
+        <v>562</v>
+      </c>
+      <c r="Y97">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A16:X33">
-    <cfRule type="expression" dxfId="70" priority="68">
+    <cfRule type="expression" dxfId="91" priority="89">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="71">
+    <cfRule type="expression" dxfId="90" priority="92">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="68" priority="67">
+    <cfRule type="expression" dxfId="89" priority="88">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="70">
+    <cfRule type="expression" dxfId="88" priority="91">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="66" priority="69">
+    <cfRule type="expression" dxfId="87" priority="90">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="65" priority="66">
+    <cfRule type="expression" dxfId="86" priority="87">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="expression" dxfId="64" priority="65">
+    <cfRule type="expression" dxfId="85" priority="86">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="63" priority="64">
+    <cfRule type="expression" dxfId="84" priority="85">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="83" priority="82">
+      <formula>$N73=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="84">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="81" priority="83">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W74 Y74">
+    <cfRule type="expression" dxfId="80" priority="79">
+      <formula>$N74=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="81">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W74 Y74">
+    <cfRule type="expression" dxfId="78" priority="80">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+    <cfRule type="expression" dxfId="77" priority="76">
+      <formula>$N75=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="78">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+    <cfRule type="expression" dxfId="75" priority="77">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N79">
+    <cfRule type="expression" dxfId="74" priority="73">
+      <formula>$N79=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="75">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N79">
+    <cfRule type="expression" dxfId="72" priority="74">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O79:W79">
+    <cfRule type="expression" dxfId="71" priority="70">
+      <formula>$N79=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="72">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O79:W79">
+    <cfRule type="expression" dxfId="69" priority="71">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N80">
+    <cfRule type="expression" dxfId="68" priority="67">
+      <formula>$N80=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="69">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N80">
+    <cfRule type="expression" dxfId="66" priority="68">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O80:W80">
+    <cfRule type="expression" dxfId="65" priority="64">
+      <formula>$N80=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="66">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O80:W80">
+    <cfRule type="expression" dxfId="63" priority="65">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="62" priority="61">
-      <formula>$N73=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="61" priority="63">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O73:W73 Y73">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="60" priority="62">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W74 Y74">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="59" priority="58">
-      <formula>$N74=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="58" priority="60">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W74 Y74">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="57" priority="59">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+  <conditionalFormatting sqref="N82">
     <cfRule type="expression" dxfId="56" priority="55">
-      <formula>$N75=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="55" priority="57">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+  <conditionalFormatting sqref="N82">
     <cfRule type="expression" dxfId="54" priority="56">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="O82:W82">
     <cfRule type="expression" dxfId="53" priority="52">
-      <formula>$N79=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="52" priority="54">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="O82:W82">
     <cfRule type="expression" dxfId="51" priority="53">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="Y83:Y97">
     <cfRule type="expression" dxfId="50" priority="49">
-      <formula>$N79=0</formula>
+      <formula>$N83=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="49" priority="51">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="Y83:Y97">
     <cfRule type="expression" dxfId="48" priority="50">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="47" priority="46">
-      <formula>$N80=0</formula>
+      <formula>$N83=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="46" priority="48">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="45" priority="47">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="44" priority="43">
-      <formula>$N80=0</formula>
+      <formula>$N84=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="43" priority="45">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="42" priority="44">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="41" priority="40">
-      <formula>$N81=0</formula>
+      <formula>$N85=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="40" priority="42">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="39" priority="41">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="38" priority="37">
-      <formula>$N81=0</formula>
+      <formula>$N86=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="37" priority="39">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="36" priority="38">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
+  <conditionalFormatting sqref="O87:V87">
     <cfRule type="expression" dxfId="35" priority="34">
-      <formula>$N82=0</formula>
+      <formula>$N87=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
+  <conditionalFormatting sqref="O87:V87">
     <cfRule type="expression" dxfId="33" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:W82">
+  <conditionalFormatting sqref="O88:W88 W89">
     <cfRule type="expression" dxfId="32" priority="31">
-      <formula>$N82=0</formula>
+      <formula>$N88=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="31" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:W82">
+  <conditionalFormatting sqref="O88:W88 W89">
     <cfRule type="expression" dxfId="30" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y83:Y91">
+  <conditionalFormatting sqref="O89:V89">
     <cfRule type="expression" dxfId="29" priority="28">
-      <formula>$N83=0</formula>
+      <formula>$N89=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="30">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y83:Y91">
+  <conditionalFormatting sqref="O89:V89">
     <cfRule type="expression" dxfId="27" priority="29">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O83:V83">
+  <conditionalFormatting sqref="O90:W90 W91">
     <cfRule type="expression" dxfId="26" priority="25">
-      <formula>$N83=0</formula>
+      <formula>$N90=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="27">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O83:V83">
+  <conditionalFormatting sqref="O90:W90 W91">
     <cfRule type="expression" dxfId="24" priority="26">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:V84">
+  <conditionalFormatting sqref="O91:V91">
     <cfRule type="expression" dxfId="23" priority="22">
-      <formula>$N84=0</formula>
+      <formula>$N91=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="24">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:V84">
+  <conditionalFormatting sqref="O91:V91">
     <cfRule type="expression" dxfId="21" priority="23">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O85:V85">
+  <conditionalFormatting sqref="O92:W92">
     <cfRule type="expression" dxfId="20" priority="19">
-      <formula>$N85=0</formula>
+      <formula>$N92=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="21">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O85:V85">
+  <conditionalFormatting sqref="O92:W92">
     <cfRule type="expression" dxfId="18" priority="20">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O93:V93">
     <cfRule type="expression" dxfId="17" priority="16">
-      <formula>$N86=0</formula>
+      <formula>$N93=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="18">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O93:V93">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:V87">
+  <conditionalFormatting sqref="O94:W94">
     <cfRule type="expression" dxfId="14" priority="13">
-      <formula>$N87=0</formula>
+      <formula>$N94=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:V87">
+  <conditionalFormatting sqref="O94:W94">
     <cfRule type="expression" dxfId="12" priority="14">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O88:W88 W89">
+  <conditionalFormatting sqref="O95:W95">
     <cfRule type="expression" dxfId="11" priority="10">
-      <formula>$N88=0</formula>
+      <formula>$N95=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O88:W88 W89">
+  <conditionalFormatting sqref="O95:W95">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="8" priority="7">
-      <formula>$N89=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O90:W90 W91">
+  <conditionalFormatting sqref="O96:V96">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N90=0</formula>
+      <formula>$N96=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O90:W90 W91">
+  <conditionalFormatting sqref="O96:V96">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:V91">
+  <conditionalFormatting sqref="O97:W97">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N91=0</formula>
+      <formula>$N97=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:V91">
+  <conditionalFormatting sqref="O97:W97">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
revised the orbit numbers, added several AR targets, added some exposures we had missed in the list of AR datasets
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDE8856-29F2-304A-B410-8746D3E34039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D852F47B-762B-8744-B148-8CED85789491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="460" windowWidth="23460" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2600" yWindow="460" windowWidth="29840" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="669">
   <si>
     <t>2MASS</t>
   </si>
@@ -1718,13 +1718,331 @@
   </si>
   <si>
     <t>STIS/G140M-STIS/G140L-STIS/E230M-STIS/G230L-STIS/G430L</t>
+  </si>
+  <si>
+    <t>V836 Tau</t>
+  </si>
+  <si>
+    <t>05h03m06.62s</t>
+  </si>
+  <si>
+    <t>+25d23m19.6s</t>
+  </si>
+  <si>
+    <t>HBC 429</t>
+  </si>
+  <si>
+    <t>J05030659+2523197</t>
+  </si>
+  <si>
+    <t>8157|11616</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-STIS/E140M-STIS/E230M-STIS/G230L-STIS/G430L</t>
+  </si>
+  <si>
+    <t>2MASS-J15570234-1950419</t>
+  </si>
+  <si>
+    <t>J15570234-1950419</t>
+  </si>
+  <si>
+    <t>15h57m02.359s</t>
+  </si>
+  <si>
+    <t>-19d50m42.03s</t>
+  </si>
+  <si>
+    <t>upper Scorpius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSC 06195􏰆00768 </t>
+  </si>
+  <si>
+    <t>COS/G130M</t>
+  </si>
+  <si>
+    <t>V397 Aur</t>
+  </si>
+  <si>
+    <t>04h56m02.03s</t>
+  </si>
+  <si>
+    <t>+30d21m03.67s</t>
+  </si>
+  <si>
+    <t>HBC 427</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-STIS/G140L-STIS/E230M-STIS/G230L-STIS/G430L</t>
+  </si>
+  <si>
+    <t>J04560201+3021037</t>
+  </si>
+  <si>
+    <t>Kraus+2008</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Ingleby+2013</t>
+  </si>
+  <si>
+    <t>K7+M2</t>
+  </si>
+  <si>
+    <t>HD142527</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-STIS/G140M</t>
+  </si>
+  <si>
+    <t>13032|14703</t>
+  </si>
+  <si>
+    <t>J15564188-4219232</t>
+  </si>
+  <si>
+    <t>15h56m41.888s</t>
+  </si>
+  <si>
+    <t>-42d19m23.25s</t>
+  </si>
+  <si>
+    <t>Mendigutia+2014</t>
+  </si>
+  <si>
+    <t>F6-7III</t>
+  </si>
+  <si>
+    <t>HD169142</t>
+  </si>
+  <si>
+    <t>18h24m29.78s</t>
+  </si>
+  <si>
+    <t>-29d46m49.91s</t>
+  </si>
+  <si>
+    <t>J18242978-2946492</t>
+  </si>
+  <si>
+    <t>12996|13032</t>
+  </si>
+  <si>
+    <t>COS/G130M-STIS/E140M-STIS/G140M-STIS/G230LB</t>
+  </si>
+  <si>
+    <t>wagner+2015</t>
+  </si>
+  <si>
+    <t>A7V</t>
+  </si>
+  <si>
+    <t>HK Ori</t>
+  </si>
+  <si>
+    <t>05h31m28.05s</t>
+  </si>
+  <si>
+    <t>+12d09m10.15s</t>
+  </si>
+  <si>
+    <t>J05312805+1209102</t>
+  </si>
+  <si>
+    <t>HBC 94</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-COS/G230L-STIS/E230M</t>
+  </si>
+  <si>
+    <t>12996|15070</t>
+  </si>
+  <si>
+    <t>Orion</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Mendigutia+2011|Donehew+2011</t>
+  </si>
+  <si>
+    <t>04h30m03.996s</t>
+  </si>
+  <si>
+    <t>+18d13m49.4355s</t>
+  </si>
+  <si>
+    <t>HD285846</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-STIS/E230M-STIS/G230L-STIS/G430L</t>
+  </si>
+  <si>
+    <t>Ardila+2013|ingleby+2013</t>
+  </si>
+  <si>
+    <t>costigan+2014</t>
+  </si>
+  <si>
+    <t>UX Tau A</t>
+  </si>
+  <si>
+    <t>Wa Oph 2</t>
+  </si>
+  <si>
+    <t>V1001 Sco A</t>
+  </si>
+  <si>
+    <t>16h11m59.27s</t>
+  </si>
+  <si>
+    <t>-19d06m53.316s</t>
+  </si>
+  <si>
+    <t>J16115927-1906532</t>
+  </si>
+  <si>
+    <t>ansdell2018</t>
+  </si>
+  <si>
+    <t>Ansdell+2018</t>
+  </si>
+  <si>
+    <t>CVSO 35</t>
+  </si>
+  <si>
+    <t>OB1A 1192</t>
+  </si>
+  <si>
+    <t>05h25m45.914s</t>
+  </si>
+  <si>
+    <t>+01d45m50.11s</t>
+  </si>
+  <si>
+    <t>J05254589+0145500</t>
+  </si>
+  <si>
+    <t>France+2017</t>
+  </si>
+  <si>
+    <t>J05265537+0140224</t>
+  </si>
+  <si>
+    <t>OB1A 1630</t>
+  </si>
+  <si>
+    <t>05h26m55.37s</t>
+  </si>
+  <si>
+    <t>+01d40m22.40s</t>
+  </si>
+  <si>
+    <t>KISO-A-0903 134</t>
+  </si>
+  <si>
+    <t>Kiso A-0903 109</t>
+  </si>
+  <si>
+    <t>CVSO 206</t>
+  </si>
+  <si>
+    <t>J05244103+0154386</t>
+  </si>
+  <si>
+    <t>05h24m41.04s</t>
+  </si>
+  <si>
+    <t>+01d54m38.53s</t>
+  </si>
+  <si>
+    <t>[PGZ2001] J161031.9-191305</t>
+  </si>
+  <si>
+    <t>J16103196-1913062</t>
+  </si>
+  <si>
+    <t>-19d13m06.08s</t>
+  </si>
+  <si>
+    <t>16h10m31.95s</t>
+  </si>
+  <si>
+    <t>lachapelle2015</t>
+  </si>
+  <si>
+    <t>[PZ99] J161019.1-250230</t>
+  </si>
+  <si>
+    <t>J16101918-2502301</t>
+  </si>
+  <si>
+    <t>16h10m19.189s</t>
+  </si>
+  <si>
+    <t>-25d02m30.22s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1 </t>
+  </si>
+  <si>
+    <t>Wahhaj+2010</t>
+  </si>
+  <si>
+    <t>RR Tau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COS/G130M-COS/G160M-COS/G230L </t>
+  </si>
+  <si>
+    <t>J05393051+2622269</t>
+  </si>
+  <si>
+    <t>+26d22m26.97s</t>
+  </si>
+  <si>
+    <t>05h39m30.51s</t>
+  </si>
+  <si>
+    <t>HBC 170</t>
+  </si>
+  <si>
+    <t>A2-3IIIe</t>
+  </si>
+  <si>
+    <t>Mendigutia+2012|Wheelwright+2010</t>
+  </si>
+  <si>
+    <t>2MASS J04390163+2336029</t>
+  </si>
+  <si>
+    <t>J04390163+2336029</t>
+  </si>
+  <si>
+    <t>+23d36m02.96s</t>
+  </si>
+  <si>
+    <t>04h39m01.63s</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>[SCH2006b] J0439016+2336030</t>
+  </si>
+  <si>
+    <t>Herczeg+2008|Yang+2012</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1862,6 +2180,21 @@
     <font>
       <sz val="12"/>
       <color rgb="FF010101"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2164,7 +2497,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2207,8 +2540,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
@@ -2222,8 +2556,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2257,6 +2595,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2267,7 +2606,307 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="122">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3498,17 +4137,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y97"/>
+  <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="108" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="108" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A26" sqref="A26"/>
-      <selection pane="topRight" activeCell="Y99" sqref="Y99"/>
+      <selection activeCell="A48" sqref="A48"/>
+      <selection pane="topRight" activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="15" max="15" width="3.1640625" customWidth="1"/>
     <col min="16" max="17" width="12.5" customWidth="1"/>
@@ -3517,7 +4157,7 @@
     <col min="24" max="24" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>459</v>
       </c>
@@ -3593,8 +4233,11 @@
       <c r="Y1" t="s">
         <v>452</v>
       </c>
+      <c r="Z1" t="s">
+        <v>584</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -3675,7 +4318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -3733,11 +4376,11 @@
         <v>0.32</v>
       </c>
       <c r="T3" s="1">
-        <f t="shared" ref="T3:T66" si="1">ROUND(R3+0.3,0)</f>
+        <f t="shared" ref="T3:T63" si="1">ROUND(R3+0.3,0)</f>
         <v>2</v>
       </c>
       <c r="U3" s="1">
-        <f t="shared" ref="U3:U66" si="2">CEILING(S3,1)</f>
+        <f t="shared" ref="U3:U65" si="2">CEILING(S3,1)</f>
         <v>1</v>
       </c>
       <c r="V3" s="1">
@@ -3752,7 +4395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -3831,7 +4474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>376</v>
       </c>
@@ -3909,7 +4552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>379</v>
       </c>
@@ -3988,7 +4631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -4065,7 +4708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -4142,7 +4785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>368</v>
       </c>
@@ -4221,7 +4864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -4298,7 +4941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -4375,7 +5018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -4454,7 +5097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>70</v>
       </c>
@@ -4533,7 +5176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>74</v>
       </c>
@@ -4610,7 +5253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>369</v>
       </c>
@@ -4684,7 +5327,7 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>83</v>
       </c>
@@ -7495,8 +8138,7 @@
         <v>0.24</v>
       </c>
       <c r="T53" s="9">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U53" s="9">
         <f t="shared" si="2"/>
@@ -7504,7 +8146,7 @@
       </c>
       <c r="V53" s="9">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W53" s="10">
         <v>16859</v>
@@ -7569,16 +8211,14 @@
         <v>0.26</v>
       </c>
       <c r="T54" s="9">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U54" s="9">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V54" s="9">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W54" s="9">
         <v>16853</v>
@@ -7721,8 +8361,7 @@
         <v>0.3</v>
       </c>
       <c r="T56" s="9">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U56" s="9">
         <f t="shared" si="2"/>
@@ -7730,7 +8369,7 @@
       </c>
       <c r="V56" s="9">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W56" s="9">
         <v>16853</v>
@@ -7877,12 +8516,11 @@
         <v>5</v>
       </c>
       <c r="U58" s="9">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V58" s="9">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W58" s="9">
         <v>16856</v>
@@ -7949,8 +8587,7 @@
         <v>0.3</v>
       </c>
       <c r="T59" s="9">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U59" s="9">
         <f t="shared" si="2"/>
@@ -7958,7 +8595,7 @@
       </c>
       <c r="V59" s="9">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W59" s="9">
         <v>16855</v>
@@ -8025,16 +8662,14 @@
         <v>0.41</v>
       </c>
       <c r="T60" s="9">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U60" s="9">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V60" s="9">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="W60" s="9">
         <v>16855</v>
@@ -8101,16 +8736,14 @@
         <v>0.38</v>
       </c>
       <c r="T61" s="9">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U61" s="9">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V61" s="9">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W61" s="9">
         <v>16858</v>
@@ -8177,8 +8810,7 @@
         <v>0.22</v>
       </c>
       <c r="T62" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U62" s="9">
         <f t="shared" si="2"/>
@@ -8186,7 +8818,7 @@
       </c>
       <c r="V62" s="9">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="W62" s="9">
         <v>16854</v>
@@ -8323,8 +8955,7 @@
         <v>0.31</v>
       </c>
       <c r="T64" s="9">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U64" s="9">
         <f t="shared" si="2"/>
@@ -8332,14 +8963,14 @@
       </c>
       <c r="V64" s="9">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W64" s="9">
         <v>16859</v>
       </c>
       <c r="X64" s="9"/>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>331</v>
       </c>
@@ -8399,8 +9030,7 @@
         <v>0.39</v>
       </c>
       <c r="T65" s="9">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="U65" s="9">
         <f t="shared" si="2"/>
@@ -8408,14 +9038,14 @@
       </c>
       <c r="V65" s="9">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W65" s="9">
         <v>16854</v>
       </c>
       <c r="X65" s="9"/>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
         <v>336</v>
       </c>
@@ -8475,23 +9105,21 @@
         <v>0.5</v>
       </c>
       <c r="T66" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U66" s="9">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V66" s="9">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="W66" s="9">
         <v>16858</v>
       </c>
       <c r="X66" s="9"/>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>341</v>
       </c>
@@ -8551,23 +9179,21 @@
         <v>0.48</v>
       </c>
       <c r="T67" s="9">
-        <f t="shared" ref="T67" si="8">ROUND(R67+0.3,0)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="U67" s="9">
-        <f t="shared" ref="U67:U69" si="9">CEILING(S67,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V67" s="9">
-        <f t="shared" ref="V67:V68" si="10">(T67+U67)*N67</f>
-        <v>14</v>
+        <f t="shared" ref="V67:V68" si="8">(T67+U67)*N67</f>
+        <v>17</v>
       </c>
       <c r="W67" s="9">
         <v>16856</v>
       </c>
       <c r="X67" s="9"/>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>346</v>
       </c>
@@ -8633,7 +9259,7 @@
         <v>9</v>
       </c>
       <c r="V68" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="W68" s="9">
@@ -8641,7 +9267,7 @@
       </c>
       <c r="X68" s="9"/>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>376</v>
       </c>
@@ -8704,11 +9330,11 @@
         <v>3</v>
       </c>
       <c r="U69" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="U69" si="9">CEILING(S69,1)</f>
         <v>1</v>
       </c>
       <c r="V69" s="7">
-        <f t="shared" ref="V69" si="11">O69+P69</f>
+        <f t="shared" ref="V69" si="10">O69+P69</f>
         <v>4</v>
       </c>
       <c r="W69" s="7">
@@ -8717,7 +9343,7 @@
       <c r="X69" s="7"/>
       <c r="Y69" s="7"/>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>377</v>
       </c>
@@ -8788,7 +9414,7 @@
       <c r="X70" s="7"/>
       <c r="Y70" s="7"/>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>378</v>
       </c>
@@ -8848,10 +9474,10 @@
         <v>0</v>
       </c>
       <c r="U71" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V71" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W71" s="7">
         <v>16596</v>
@@ -8859,7 +9485,7 @@
       <c r="X71" s="7"/>
       <c r="Y71" s="7"/>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>384</v>
       </c>
@@ -8935,8 +9561,11 @@
       <c r="Y72">
         <v>3</v>
       </c>
+      <c r="Z72" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>390</v>
       </c>
@@ -9012,8 +9641,11 @@
       <c r="Y73">
         <v>3</v>
       </c>
+      <c r="Z73" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>395</v>
       </c>
@@ -9089,8 +9721,11 @@
       <c r="Y74">
         <v>3</v>
       </c>
+      <c r="Z74" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>401</v>
       </c>
@@ -9166,8 +9801,11 @@
       <c r="Y75">
         <v>3</v>
       </c>
+      <c r="Z75" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>408</v>
       </c>
@@ -9243,8 +9881,11 @@
       <c r="Y76">
         <v>3</v>
       </c>
+      <c r="Z76" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>414</v>
       </c>
@@ -9320,8 +9961,11 @@
       <c r="Y77">
         <v>3</v>
       </c>
+      <c r="Z77" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>419</v>
       </c>
@@ -9397,8 +10041,11 @@
       <c r="Y78">
         <v>3</v>
       </c>
+      <c r="Z78" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>425</v>
       </c>
@@ -9474,8 +10121,11 @@
       <c r="Y79">
         <v>3</v>
       </c>
+      <c r="Z79" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>433</v>
       </c>
@@ -9551,8 +10201,11 @@
       <c r="Y80">
         <v>3</v>
       </c>
+      <c r="Z80" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>439</v>
       </c>
@@ -9628,8 +10281,11 @@
       <c r="Y81">
         <v>3</v>
       </c>
+      <c r="Z81" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>446</v>
       </c>
@@ -9705,8 +10361,11 @@
       <c r="Y82">
         <v>3</v>
       </c>
+      <c r="Z82" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>469</v>
       </c>
@@ -9779,8 +10438,11 @@
       <c r="Y83">
         <v>3</v>
       </c>
+      <c r="Z83" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>476</v>
       </c>
@@ -9850,8 +10512,11 @@
       <c r="Y84">
         <v>3</v>
       </c>
+      <c r="Z84" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>483</v>
       </c>
@@ -9918,8 +10583,11 @@
       <c r="Y85">
         <v>3</v>
       </c>
+      <c r="Z85" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>488</v>
       </c>
@@ -9995,8 +10663,11 @@
       <c r="Y86">
         <v>3</v>
       </c>
+      <c r="Z86" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>495</v>
       </c>
@@ -10069,8 +10740,11 @@
       <c r="Y87">
         <v>3</v>
       </c>
+      <c r="Z87" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>502</v>
       </c>
@@ -10134,8 +10808,11 @@
       <c r="Y88">
         <v>3</v>
       </c>
+      <c r="Z88" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>504</v>
       </c>
@@ -10211,8 +10888,11 @@
       <c r="Y89">
         <v>3</v>
       </c>
+      <c r="Z89" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>510</v>
       </c>
@@ -10288,8 +10968,11 @@
       <c r="Y90">
         <v>3</v>
       </c>
+      <c r="Z90" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>513</v>
       </c>
@@ -10362,8 +11045,11 @@
       <c r="Y91">
         <v>3</v>
       </c>
+      <c r="Z91" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>525</v>
       </c>
@@ -10440,7 +11126,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>531</v>
       </c>
@@ -10513,8 +11199,11 @@
       <c r="Y93">
         <v>5</v>
       </c>
+      <c r="Z93" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>538</v>
       </c>
@@ -10584,8 +11273,11 @@
       <c r="Y94">
         <v>5</v>
       </c>
+      <c r="Z94" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>549</v>
       </c>
@@ -10658,8 +11350,11 @@
       <c r="Y95">
         <v>5</v>
       </c>
+      <c r="Z95" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>553</v>
       </c>
@@ -10724,8 +11419,11 @@
       <c r="Y96">
         <v>5</v>
       </c>
+      <c r="Z96" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>559</v>
       </c>
@@ -10739,7 +11437,7 @@
         <v>82</v>
       </c>
       <c r="G97">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H97" t="s">
         <v>51</v>
@@ -10791,396 +11489,1592 @@
       </c>
       <c r="Y97">
         <v>5</v>
+      </c>
+      <c r="Z97" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>563</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="C98" t="s">
+        <v>566</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G98">
+        <v>140</v>
+      </c>
+      <c r="H98" t="s">
+        <v>25</v>
+      </c>
+      <c r="I98">
+        <v>0.8</v>
+      </c>
+      <c r="J98">
+        <v>-8.9600000000000009</v>
+      </c>
+      <c r="K98">
+        <v>1.5</v>
+      </c>
+      <c r="M98">
+        <v>13.49</v>
+      </c>
+      <c r="N98">
+        <v>2</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="Q98">
+        <v>0</v>
+      </c>
+      <c r="R98">
+        <v>0</v>
+      </c>
+      <c r="S98">
+        <v>0</v>
+      </c>
+      <c r="T98">
+        <v>0</v>
+      </c>
+      <c r="U98">
+        <v>0</v>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+      <c r="W98" t="s">
+        <v>568</v>
+      </c>
+      <c r="X98" t="s">
+        <v>569</v>
+      </c>
+      <c r="Y98">
+        <v>5</v>
+      </c>
+      <c r="Z98" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>577</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="C99" t="s">
+        <v>580</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>579</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G99">
+        <v>140</v>
+      </c>
+      <c r="H99" t="s">
+        <v>586</v>
+      </c>
+      <c r="I99">
+        <v>0.8</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>11.72</v>
+      </c>
+      <c r="N99">
+        <v>2</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <v>0</v>
+      </c>
+      <c r="R99">
+        <v>0</v>
+      </c>
+      <c r="S99">
+        <v>0</v>
+      </c>
+      <c r="T99">
+        <v>0</v>
+      </c>
+      <c r="U99">
+        <v>0</v>
+      </c>
+      <c r="V99">
+        <v>0</v>
+      </c>
+      <c r="W99" t="s">
+        <v>487</v>
+      </c>
+      <c r="X99" t="s">
+        <v>581</v>
+      </c>
+      <c r="Y99">
+        <v>5</v>
+      </c>
+      <c r="Z99" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>587</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>592</v>
+      </c>
+      <c r="F100" s="12"/>
+      <c r="G100">
+        <v>140</v>
+      </c>
+      <c r="H100" t="s">
+        <v>594</v>
+      </c>
+      <c r="I100">
+        <v>2</v>
+      </c>
+      <c r="J100">
+        <v>-6.7</v>
+      </c>
+      <c r="K100">
+        <v>0.78</v>
+      </c>
+      <c r="M100">
+        <v>8.34</v>
+      </c>
+      <c r="N100">
+        <v>2</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+      <c r="P100">
+        <v>2</v>
+      </c>
+      <c r="Q100">
+        <v>0</v>
+      </c>
+      <c r="R100">
+        <v>0</v>
+      </c>
+      <c r="S100">
+        <v>0</v>
+      </c>
+      <c r="T100">
+        <v>0</v>
+      </c>
+      <c r="U100">
+        <v>0</v>
+      </c>
+      <c r="V100">
+        <v>0</v>
+      </c>
+      <c r="W100" t="s">
+        <v>589</v>
+      </c>
+      <c r="X100" t="s">
+        <v>588</v>
+      </c>
+      <c r="Y100">
+        <v>5</v>
+      </c>
+      <c r="Z100" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>595</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="E101" s="15" t="s">
+        <v>597</v>
+      </c>
+      <c r="F101" s="12"/>
+      <c r="G101">
+        <v>145</v>
+      </c>
+      <c r="H101" t="s">
+        <v>602</v>
+      </c>
+      <c r="I101">
+        <v>1.65</v>
+      </c>
+      <c r="J101">
+        <v>-8.68</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="M101">
+        <v>8.16</v>
+      </c>
+      <c r="N101">
+        <v>2</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+      <c r="P101">
+        <v>2</v>
+      </c>
+      <c r="Q101">
+        <v>0</v>
+      </c>
+      <c r="R101">
+        <v>0</v>
+      </c>
+      <c r="S101">
+        <v>0</v>
+      </c>
+      <c r="T101">
+        <v>0</v>
+      </c>
+      <c r="U101">
+        <v>0</v>
+      </c>
+      <c r="V101">
+        <v>0</v>
+      </c>
+      <c r="W101" t="s">
+        <v>599</v>
+      </c>
+      <c r="X101" t="s">
+        <v>600</v>
+      </c>
+      <c r="Y101">
+        <v>5</v>
+      </c>
+      <c r="Z101" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>603</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="C102" t="s">
+        <v>607</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="F102" s="12" t="s">
+        <v>610</v>
+      </c>
+      <c r="G102">
+        <v>460</v>
+      </c>
+      <c r="H102" t="s">
+        <v>611</v>
+      </c>
+      <c r="I102">
+        <v>3</v>
+      </c>
+      <c r="J102">
+        <v>-5.24</v>
+      </c>
+      <c r="K102">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L102">
+        <v>11.82</v>
+      </c>
+      <c r="M102">
+        <v>12.06</v>
+      </c>
+      <c r="N102">
+        <v>2</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+      <c r="P102">
+        <v>2</v>
+      </c>
+      <c r="Q102">
+        <v>0</v>
+      </c>
+      <c r="R102">
+        <v>0</v>
+      </c>
+      <c r="S102">
+        <v>0</v>
+      </c>
+      <c r="T102">
+        <v>0</v>
+      </c>
+      <c r="U102">
+        <v>0</v>
+      </c>
+      <c r="V102">
+        <v>0</v>
+      </c>
+      <c r="W102" t="s">
+        <v>609</v>
+      </c>
+      <c r="X102" t="s">
+        <v>608</v>
+      </c>
+      <c r="Y102">
+        <v>5</v>
+      </c>
+      <c r="Z102" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>619</v>
+      </c>
+      <c r="B103" s="5"/>
+      <c r="C103" t="s">
+        <v>615</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="F103" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G103">
+        <v>140</v>
+      </c>
+      <c r="H103" t="s">
+        <v>217</v>
+      </c>
+      <c r="I103">
+        <v>1.3</v>
+      </c>
+      <c r="J103">
+        <v>-7.3250000000000002</v>
+      </c>
+      <c r="L103">
+        <v>11.23</v>
+      </c>
+      <c r="M103">
+        <v>10.8</v>
+      </c>
+      <c r="N103">
+        <v>2</v>
+      </c>
+      <c r="O103">
+        <v>0</v>
+      </c>
+      <c r="P103">
+        <v>2</v>
+      </c>
+      <c r="Q103">
+        <v>0</v>
+      </c>
+      <c r="R103">
+        <v>0</v>
+      </c>
+      <c r="S103">
+        <v>0</v>
+      </c>
+      <c r="T103">
+        <v>0</v>
+      </c>
+      <c r="U103">
+        <v>0</v>
+      </c>
+      <c r="V103">
+        <v>0</v>
+      </c>
+      <c r="W103">
+        <v>11616</v>
+      </c>
+      <c r="X103" t="s">
+        <v>616</v>
+      </c>
+      <c r="Z103" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>620</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="C104" t="s">
+        <v>621</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="E104" s="13" t="s">
+        <v>623</v>
+      </c>
+      <c r="F104" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="G104">
+        <v>145</v>
+      </c>
+      <c r="H104" t="s">
+        <v>249</v>
+      </c>
+      <c r="M104">
+        <v>11.66</v>
+      </c>
+      <c r="N104">
+        <v>2</v>
+      </c>
+      <c r="O104">
+        <v>0</v>
+      </c>
+      <c r="P104">
+        <v>2</v>
+      </c>
+      <c r="Q104">
+        <v>0</v>
+      </c>
+      <c r="R104">
+        <v>0</v>
+      </c>
+      <c r="S104">
+        <v>0</v>
+      </c>
+      <c r="T104">
+        <v>0</v>
+      </c>
+      <c r="U104">
+        <v>0</v>
+      </c>
+      <c r="V104">
+        <v>0</v>
+      </c>
+      <c r="W104">
+        <v>15310</v>
+      </c>
+      <c r="X104" t="s">
+        <v>576</v>
+      </c>
+      <c r="Y104">
+        <v>5</v>
+      </c>
+      <c r="Z104" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>570</v>
+      </c>
+      <c r="B105" t="s">
+        <v>571</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>575</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>573</v>
+      </c>
+      <c r="F105" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="G105">
+        <v>145</v>
+      </c>
+      <c r="H105" t="s">
+        <v>25</v>
+      </c>
+      <c r="I105">
+        <v>0.77</v>
+      </c>
+      <c r="M105">
+        <v>11.67</v>
+      </c>
+      <c r="N105">
+        <v>2</v>
+      </c>
+      <c r="O105">
+        <v>0</v>
+      </c>
+      <c r="P105">
+        <v>0</v>
+      </c>
+      <c r="Q105">
+        <v>0</v>
+      </c>
+      <c r="R105">
+        <v>0</v>
+      </c>
+      <c r="S105">
+        <v>0</v>
+      </c>
+      <c r="T105">
+        <v>0</v>
+      </c>
+      <c r="U105">
+        <v>0</v>
+      </c>
+      <c r="V105">
+        <v>0</v>
+      </c>
+      <c r="W105">
+        <v>15310</v>
+      </c>
+      <c r="X105" t="s">
+        <v>576</v>
+      </c>
+      <c r="Y105">
+        <v>5</v>
+      </c>
+      <c r="Z105" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>627</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="E106" s="13" t="s">
+        <v>630</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G106">
+        <v>450</v>
+      </c>
+      <c r="H106" t="s">
+        <v>25</v>
+      </c>
+      <c r="I106">
+        <v>0.77</v>
+      </c>
+      <c r="J106">
+        <v>-8.77</v>
+      </c>
+      <c r="K106">
+        <v>0.85</v>
+      </c>
+      <c r="M106">
+        <v>13.36</v>
+      </c>
+      <c r="N106">
+        <v>2</v>
+      </c>
+      <c r="O106">
+        <v>0</v>
+      </c>
+      <c r="P106">
+        <v>0</v>
+      </c>
+      <c r="Q106">
+        <v>0</v>
+      </c>
+      <c r="R106">
+        <v>0</v>
+      </c>
+      <c r="S106">
+        <v>0</v>
+      </c>
+      <c r="T106">
+        <v>0</v>
+      </c>
+      <c r="U106">
+        <v>0</v>
+      </c>
+      <c r="V106">
+        <v>0</v>
+      </c>
+      <c r="W106">
+        <v>13363</v>
+      </c>
+      <c r="X106" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y106">
+        <v>5</v>
+      </c>
+      <c r="Z106" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A107" s="14" t="s">
+        <v>637</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>634</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="E107" s="13" t="s">
+        <v>636</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G107">
+        <v>450</v>
+      </c>
+      <c r="I107">
+        <v>0.4</v>
+      </c>
+      <c r="J107">
+        <v>-9.1</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="M107">
+        <v>15.56</v>
+      </c>
+      <c r="N107">
+        <v>2</v>
+      </c>
+      <c r="O107">
+        <v>0</v>
+      </c>
+      <c r="P107">
+        <v>0</v>
+      </c>
+      <c r="Q107">
+        <v>0</v>
+      </c>
+      <c r="R107">
+        <v>0</v>
+      </c>
+      <c r="S107">
+        <v>0</v>
+      </c>
+      <c r="T107">
+        <v>0</v>
+      </c>
+      <c r="U107">
+        <v>0</v>
+      </c>
+      <c r="V107">
+        <v>0</v>
+      </c>
+      <c r="W107">
+        <v>13363</v>
+      </c>
+      <c r="X107" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y107">
+        <v>5</v>
+      </c>
+      <c r="Z107" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="E108" s="13" t="s">
+        <v>642</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G108">
+        <v>450</v>
+      </c>
+      <c r="I108">
+        <v>0.8</v>
+      </c>
+      <c r="J108">
+        <v>-8.1300000000000008</v>
+      </c>
+      <c r="K108">
+        <v>0.6</v>
+      </c>
+      <c r="M108">
+        <v>14.93</v>
+      </c>
+      <c r="N108">
+        <v>2</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
+      </c>
+      <c r="P108">
+        <v>0</v>
+      </c>
+      <c r="Q108">
+        <v>0</v>
+      </c>
+      <c r="R108">
+        <v>0</v>
+      </c>
+      <c r="S108">
+        <v>0</v>
+      </c>
+      <c r="T108">
+        <v>0</v>
+      </c>
+      <c r="U108">
+        <v>0</v>
+      </c>
+      <c r="V108">
+        <v>0</v>
+      </c>
+      <c r="W108">
+        <v>13363</v>
+      </c>
+      <c r="X108" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y108">
+        <v>5</v>
+      </c>
+      <c r="Z108" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="E109" s="13" t="s">
+        <v>645</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="G109">
+        <v>145</v>
+      </c>
+      <c r="H109" t="s">
+        <v>25</v>
+      </c>
+      <c r="I109">
+        <v>0.77</v>
+      </c>
+      <c r="K109">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M109">
+        <v>13.56</v>
+      </c>
+      <c r="N109">
+        <v>2</v>
+      </c>
+      <c r="O109">
+        <v>0</v>
+      </c>
+      <c r="P109">
+        <v>0</v>
+      </c>
+      <c r="Q109">
+        <v>0</v>
+      </c>
+      <c r="R109">
+        <v>0</v>
+      </c>
+      <c r="S109">
+        <v>0</v>
+      </c>
+      <c r="T109">
+        <v>0</v>
+      </c>
+      <c r="U109">
+        <v>0</v>
+      </c>
+      <c r="V109">
+        <v>0</v>
+      </c>
+      <c r="W109">
+        <v>15310</v>
+      </c>
+      <c r="X109" t="s">
+        <v>576</v>
+      </c>
+      <c r="Y109">
+        <v>5</v>
+      </c>
+      <c r="Z109" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C110" s="12"/>
+      <c r="D110" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="E110" s="13" t="s">
+        <v>651</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="H110" t="s">
+        <v>652</v>
+      </c>
+      <c r="K110">
+        <v>0.3</v>
+      </c>
+      <c r="M110">
+        <v>11.98</v>
+      </c>
+      <c r="N110">
+        <v>2</v>
+      </c>
+      <c r="O110">
+        <v>0</v>
+      </c>
+      <c r="P110">
+        <v>0</v>
+      </c>
+      <c r="Q110">
+        <v>0</v>
+      </c>
+      <c r="R110">
+        <v>0</v>
+      </c>
+      <c r="S110">
+        <v>0</v>
+      </c>
+      <c r="T110">
+        <v>0</v>
+      </c>
+      <c r="U110">
+        <v>0</v>
+      </c>
+      <c r="V110">
+        <v>0</v>
+      </c>
+      <c r="W110">
+        <v>15310</v>
+      </c>
+      <c r="X110" t="s">
+        <v>576</v>
+      </c>
+      <c r="Y110">
+        <v>5</v>
+      </c>
+      <c r="Z110" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="E111" s="13" t="s">
+        <v>657</v>
+      </c>
+      <c r="G111">
+        <v>2103</v>
+      </c>
+      <c r="H111" t="s">
+        <v>660</v>
+      </c>
+      <c r="J111">
+        <v>-4.1100000000000003</v>
+      </c>
+      <c r="L111">
+        <v>11.64</v>
+      </c>
+      <c r="M111">
+        <v>12.09</v>
+      </c>
+      <c r="N111">
+        <v>2</v>
+      </c>
+      <c r="O111">
+        <v>0</v>
+      </c>
+      <c r="P111">
+        <v>0</v>
+      </c>
+      <c r="Q111">
+        <v>0</v>
+      </c>
+      <c r="R111">
+        <v>0</v>
+      </c>
+      <c r="S111">
+        <v>0</v>
+      </c>
+      <c r="T111">
+        <v>0</v>
+      </c>
+      <c r="U111">
+        <v>0</v>
+      </c>
+      <c r="V111">
+        <v>0</v>
+      </c>
+      <c r="W111">
+        <v>12996</v>
+      </c>
+      <c r="X111" t="s">
+        <v>655</v>
+      </c>
+      <c r="Y111">
+        <v>5</v>
+      </c>
+      <c r="Z111" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="C112" s="16" t="s">
+        <v>667</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="E112" s="13" t="s">
+        <v>664</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="G112">
+        <v>140</v>
+      </c>
+      <c r="H112" t="s">
+        <v>666</v>
+      </c>
+      <c r="I112">
+        <v>0.17</v>
+      </c>
+      <c r="J112">
+        <v>-9.36</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>18.3</v>
+      </c>
+      <c r="M112">
+        <v>16</v>
+      </c>
+      <c r="N112">
+        <v>2</v>
+      </c>
+      <c r="O112">
+        <v>0</v>
+      </c>
+      <c r="P112">
+        <v>0</v>
+      </c>
+      <c r="Q112">
+        <v>0</v>
+      </c>
+      <c r="R112">
+        <v>0</v>
+      </c>
+      <c r="S112">
+        <v>0</v>
+      </c>
+      <c r="T112">
+        <v>0</v>
+      </c>
+      <c r="U112">
+        <v>0</v>
+      </c>
+      <c r="V112">
+        <v>0</v>
+      </c>
+      <c r="W112">
+        <v>11616</v>
+      </c>
+      <c r="X112" t="s">
+        <v>530</v>
+      </c>
+      <c r="Y112">
+        <v>5</v>
+      </c>
+      <c r="Z112" t="s">
+        <v>668</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A16:X33">
-    <cfRule type="expression" dxfId="91" priority="89">
+    <cfRule type="expression" dxfId="121" priority="122">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="92">
+    <cfRule type="expression" dxfId="120" priority="125">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="89" priority="88">
+    <cfRule type="expression" dxfId="119" priority="121">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="91">
+    <cfRule type="expression" dxfId="118" priority="124">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="87" priority="90">
+    <cfRule type="expression" dxfId="117" priority="123">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="86" priority="87">
+    <cfRule type="expression" dxfId="116" priority="120">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="expression" dxfId="85" priority="86">
+    <cfRule type="expression" dxfId="115" priority="119">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="84" priority="85">
+    <cfRule type="expression" dxfId="114" priority="118">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="83" priority="82">
+    <cfRule type="expression" dxfId="113" priority="115">
       <formula>$N73=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="84">
+    <cfRule type="expression" dxfId="112" priority="117">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="81" priority="83">
+    <cfRule type="expression" dxfId="111" priority="116">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="80" priority="79">
+    <cfRule type="expression" dxfId="110" priority="112">
       <formula>$N74=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="81">
+    <cfRule type="expression" dxfId="109" priority="114">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="78" priority="80">
+    <cfRule type="expression" dxfId="108" priority="113">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="77" priority="76">
+    <cfRule type="expression" dxfId="107" priority="109">
       <formula>$N75=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="78">
+    <cfRule type="expression" dxfId="106" priority="111">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="75" priority="77">
+    <cfRule type="expression" dxfId="105" priority="110">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="74" priority="73">
+    <cfRule type="expression" dxfId="104" priority="106">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="75">
+    <cfRule type="expression" dxfId="103" priority="108">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="72" priority="74">
+    <cfRule type="expression" dxfId="102" priority="107">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="71" priority="70">
+    <cfRule type="expression" dxfId="101" priority="103">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="72">
+    <cfRule type="expression" dxfId="100" priority="105">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="69" priority="71">
+    <cfRule type="expression" dxfId="99" priority="104">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="68" priority="67">
+    <cfRule type="expression" dxfId="98" priority="100">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="69">
+    <cfRule type="expression" dxfId="97" priority="102">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="66" priority="68">
+    <cfRule type="expression" dxfId="96" priority="101">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="65" priority="64">
+    <cfRule type="expression" dxfId="95" priority="97">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="66">
+    <cfRule type="expression" dxfId="94" priority="99">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="63" priority="65">
+    <cfRule type="expression" dxfId="93" priority="98">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="62" priority="61">
+    <cfRule type="expression" dxfId="92" priority="94">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="63">
+    <cfRule type="expression" dxfId="91" priority="96">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="60" priority="62">
+    <cfRule type="expression" dxfId="90" priority="95">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="59" priority="58">
+    <cfRule type="expression" dxfId="89" priority="91">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="60">
+    <cfRule type="expression" dxfId="88" priority="93">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="57" priority="59">
+    <cfRule type="expression" dxfId="87" priority="92">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="56" priority="55">
+    <cfRule type="expression" dxfId="86" priority="88">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57">
+    <cfRule type="expression" dxfId="85" priority="90">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="54" priority="56">
+    <cfRule type="expression" dxfId="84" priority="89">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="53" priority="52">
+    <cfRule type="expression" dxfId="83" priority="85">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="54">
+    <cfRule type="expression" dxfId="82" priority="87">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="51" priority="53">
+    <cfRule type="expression" dxfId="81" priority="86">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y83:Y97">
-    <cfRule type="expression" dxfId="50" priority="49">
+  <conditionalFormatting sqref="Y83:Y96">
+    <cfRule type="expression" dxfId="80" priority="82">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="51">
+    <cfRule type="expression" dxfId="79" priority="84">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y83:Y97">
-    <cfRule type="expression" dxfId="48" priority="50">
+  <conditionalFormatting sqref="Y83:Y96">
+    <cfRule type="expression" dxfId="78" priority="83">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="47" priority="46">
+    <cfRule type="expression" dxfId="77" priority="79">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="48">
+    <cfRule type="expression" dxfId="76" priority="81">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="45" priority="47">
+    <cfRule type="expression" dxfId="75" priority="80">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="44" priority="43">
+    <cfRule type="expression" dxfId="74" priority="76">
       <formula>$N84=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="45">
+    <cfRule type="expression" dxfId="73" priority="78">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="42" priority="44">
+    <cfRule type="expression" dxfId="72" priority="77">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="41" priority="40">
+    <cfRule type="expression" dxfId="71" priority="73">
       <formula>$N85=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="42">
+    <cfRule type="expression" dxfId="70" priority="75">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="39" priority="41">
+    <cfRule type="expression" dxfId="69" priority="74">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
+    <cfRule type="expression" dxfId="68" priority="70">
+      <formula>$N86=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="72">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O86:V86">
+    <cfRule type="expression" dxfId="66" priority="71">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O87:V87">
+    <cfRule type="expression" dxfId="65" priority="67">
+      <formula>$N87=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="69">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O87:V87">
+    <cfRule type="expression" dxfId="63" priority="68">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O88:W88 W89">
+    <cfRule type="expression" dxfId="62" priority="64">
+      <formula>$N88=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="66">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O88:W88 W89">
+    <cfRule type="expression" dxfId="60" priority="65">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O89:V89">
+    <cfRule type="expression" dxfId="59" priority="61">
+      <formula>$N89=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="63">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O89:V89">
+    <cfRule type="expression" dxfId="57" priority="62">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O90:W90 W91">
+    <cfRule type="expression" dxfId="56" priority="58">
+      <formula>$N90=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="60">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O90:W90 W91">
+    <cfRule type="expression" dxfId="54" priority="59">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O91:V91">
+    <cfRule type="expression" dxfId="53" priority="55">
+      <formula>$N91=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="57">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O91:V91">
+    <cfRule type="expression" dxfId="51" priority="56">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O92:W92">
+    <cfRule type="expression" dxfId="50" priority="52">
+      <formula>$N92=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="54">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O92:W92">
+    <cfRule type="expression" dxfId="48" priority="53">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O93:V93">
+    <cfRule type="expression" dxfId="47" priority="49">
+      <formula>$N93=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="51">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O93:V93">
+    <cfRule type="expression" dxfId="45" priority="50">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O94:W94">
+    <cfRule type="expression" dxfId="44" priority="46">
+      <formula>$N94=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="48">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O94:W94">
+    <cfRule type="expression" dxfId="42" priority="47">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O95:W95">
+    <cfRule type="expression" dxfId="41" priority="43">
+      <formula>$N95=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="45">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O95:W95">
+    <cfRule type="expression" dxfId="39" priority="44">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O96:V96">
     <cfRule type="expression" dxfId="38" priority="37">
-      <formula>$N86=0</formula>
+      <formula>$N96=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="37" priority="39">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O96:V96">
     <cfRule type="expression" dxfId="36" priority="38">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="35" priority="34">
-      <formula>$N87=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="36">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="33" priority="35">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="32" priority="31">
-      <formula>$N88=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="33">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="30" priority="32">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="29" priority="28">
-      <formula>$N89=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="30">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="27" priority="29">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="26" priority="25">
-      <formula>$N90=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="24" priority="26">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O91:V91">
+  <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y112">
     <cfRule type="expression" dxfId="23" priority="22">
-      <formula>$N91=0</formula>
+      <formula>$N105=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="24">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:V91">
+  <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y112">
     <cfRule type="expression" dxfId="21" priority="23">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O92:W92">
+  <conditionalFormatting sqref="O106:V106">
     <cfRule type="expression" dxfId="20" priority="19">
-      <formula>$N92=0</formula>
+      <formula>$N106=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="21">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O92:W92">
+  <conditionalFormatting sqref="O106:V106">
     <cfRule type="expression" dxfId="18" priority="20">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O93:V93">
+  <conditionalFormatting sqref="O107:V107">
     <cfRule type="expression" dxfId="17" priority="16">
-      <formula>$N93=0</formula>
+      <formula>$N107=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="18">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O93:V93">
+  <conditionalFormatting sqref="O107:V107">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O94:W94">
+  <conditionalFormatting sqref="O108:V108">
     <cfRule type="expression" dxfId="14" priority="13">
-      <formula>$N94=0</formula>
+      <formula>$N108=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O94:W94">
+  <conditionalFormatting sqref="O108:V108">
     <cfRule type="expression" dxfId="12" priority="14">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O95:W95">
+  <conditionalFormatting sqref="O109:V109">
     <cfRule type="expression" dxfId="11" priority="10">
-      <formula>$N95=0</formula>
+      <formula>$N109=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O95:W95">
+  <conditionalFormatting sqref="O109:V109">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O96:V96">
+  <conditionalFormatting sqref="O110:V110">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>$N110=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O110:V110">
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O111:V111">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N96=0</formula>
+      <formula>$N111=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O96:V96">
+  <conditionalFormatting sqref="O111:V111">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O97:W97">
+  <conditionalFormatting sqref="O112:V112">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N97=0</formula>
+      <formula>$N112=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O97:W97">
+  <conditionalFormatting sqref="O112:V112">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C112" r:id="rId1" display="https://cds.unistra.fr/cgi-bin/Dic-Simbad?%5bSCH2006b%5d" xr:uid="{9DD3F2B4-9683-7B49-8C86-4938A87017D6}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more AR CTTS in the sample, added some missing exposures, added an alias for THA15-28
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D852F47B-762B-8744-B148-8CED85789491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A4E84A-D613-7740-AD48-06F2086D2EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="460" windowWidth="29840" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4100" yWindow="460" windowWidth="24480" windowHeight="18200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="704">
   <si>
     <t>2MASS</t>
   </si>
@@ -2036,6 +2036,111 @@
   </si>
   <si>
     <t>Herczeg+2008|Yang+2012</t>
+  </si>
+  <si>
+    <t>Sz102</t>
+  </si>
+  <si>
+    <t>J16082972-3903110</t>
+  </si>
+  <si>
+    <t>HBC 617</t>
+  </si>
+  <si>
+    <t>-39d03m11.024s</t>
+  </si>
+  <si>
+    <t>16h08m29.73s</t>
+  </si>
+  <si>
+    <t>9435|9807|11616|14177|15210</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-STIS/E230M-STIS/G230L-STIS/G430L-STIS/G140M-STIS/G430M-STIS/G750M</t>
+  </si>
+  <si>
+    <t>-34d17m30.64s</t>
+  </si>
+  <si>
+    <t>V HT Lup</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-COS/G140L-STIS/G230L-STIS/G230M-STIS/G430L</t>
+  </si>
+  <si>
+    <t>&gt;1.4</t>
+  </si>
+  <si>
+    <t>&lt;-8.24</t>
+  </si>
+  <si>
+    <t>T Ori</t>
+  </si>
+  <si>
+    <t>TWA 2</t>
+  </si>
+  <si>
+    <t>J11091380-3001398</t>
+  </si>
+  <si>
+    <t>CD-29 8887</t>
+  </si>
+  <si>
+    <t>-30d01m39.97s</t>
+  </si>
+  <si>
+    <t>11h09m13.79s</t>
+  </si>
+  <si>
+    <t>TWA 7</t>
+  </si>
+  <si>
+    <t>J10423011-3340162</t>
+  </si>
+  <si>
+    <t>-33d40m16.22s</t>
+  </si>
+  <si>
+    <t>10d42m30.10s</t>
+  </si>
+  <si>
+    <t>M2.2</t>
+  </si>
+  <si>
+    <t>Herczeg+2014</t>
+  </si>
+  <si>
+    <t>M3.2</t>
+  </si>
+  <si>
+    <t>Alcala+2017</t>
+  </si>
+  <si>
+    <t>Herczeg+2014|Ren+2021</t>
+  </si>
+  <si>
+    <t>CE Ant</t>
+  </si>
+  <si>
+    <t>7310|8238|12161</t>
+  </si>
+  <si>
+    <t>+25d52m30.90s</t>
+  </si>
+  <si>
+    <t>04h32m43.02s</t>
+  </si>
+  <si>
+    <t>HBC 52</t>
+  </si>
+  <si>
+    <t>UZ Tau E</t>
+  </si>
+  <si>
+    <t>Jensen+2007|Jones+2012</t>
+  </si>
+  <si>
+    <t>COS/G160M-COS/G230L</t>
   </si>
 </sst>
 </file>
@@ -2542,7 +2647,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
@@ -2560,6 +2665,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2606,7 +2712,2597 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="122">
+  <dxfs count="381">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4137,12 +6833,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z112"/>
+  <dimension ref="A1:Z122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="F111" sqref="F111"/>
+      <selection pane="topRight" activeCell="Y119" sqref="Y119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12593,487 +15289,932 @@
         <v>668</v>
       </c>
     </row>
+    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>671</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="E113" s="13" t="s">
+        <v>672</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G113">
+        <v>200</v>
+      </c>
+      <c r="H113" t="s">
+        <v>217</v>
+      </c>
+      <c r="K113">
+        <v>0.7</v>
+      </c>
+      <c r="M113">
+        <v>15.91</v>
+      </c>
+      <c r="N113">
+        <v>2</v>
+      </c>
+      <c r="O113">
+        <v>0</v>
+      </c>
+      <c r="P113">
+        <v>0</v>
+      </c>
+      <c r="Q113">
+        <v>0</v>
+      </c>
+      <c r="R113">
+        <v>0</v>
+      </c>
+      <c r="S113">
+        <v>0</v>
+      </c>
+      <c r="T113">
+        <v>0</v>
+      </c>
+      <c r="U113">
+        <v>0</v>
+      </c>
+      <c r="V113">
+        <v>0</v>
+      </c>
+      <c r="W113" t="s">
+        <v>674</v>
+      </c>
+      <c r="X113" t="s">
+        <v>675</v>
+      </c>
+      <c r="Y113">
+        <v>5</v>
+      </c>
+      <c r="Z113" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="114" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="E114" s="13" t="s">
+        <v>676</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G114">
+        <v>150</v>
+      </c>
+      <c r="H114" t="s">
+        <v>217</v>
+      </c>
+      <c r="I114" t="s">
+        <v>679</v>
+      </c>
+      <c r="J114" t="s">
+        <v>680</v>
+      </c>
+      <c r="K114">
+        <v>1</v>
+      </c>
+      <c r="L114">
+        <v>12.47</v>
+      </c>
+      <c r="M114">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="N114">
+        <v>2</v>
+      </c>
+      <c r="O114">
+        <v>0</v>
+      </c>
+      <c r="P114">
+        <v>0</v>
+      </c>
+      <c r="Q114">
+        <v>0</v>
+      </c>
+      <c r="R114">
+        <v>0</v>
+      </c>
+      <c r="S114">
+        <v>0</v>
+      </c>
+      <c r="T114">
+        <v>0</v>
+      </c>
+      <c r="U114">
+        <v>0</v>
+      </c>
+      <c r="V114">
+        <v>0</v>
+      </c>
+      <c r="W114" t="s">
+        <v>456</v>
+      </c>
+      <c r="X114" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y114">
+        <v>5</v>
+      </c>
+      <c r="Z114" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>687</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="E115" s="13" t="s">
+        <v>689</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G115">
+        <v>34</v>
+      </c>
+      <c r="H115" t="s">
+        <v>693</v>
+      </c>
+      <c r="I115">
+        <v>0.46</v>
+      </c>
+      <c r="J115">
+        <v>-12</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="M115">
+        <v>10.91</v>
+      </c>
+      <c r="N115">
+        <v>2</v>
+      </c>
+      <c r="O115">
+        <v>0</v>
+      </c>
+      <c r="P115">
+        <v>0</v>
+      </c>
+      <c r="Q115">
+        <v>0</v>
+      </c>
+      <c r="R115">
+        <v>0</v>
+      </c>
+      <c r="S115">
+        <v>0</v>
+      </c>
+      <c r="T115">
+        <v>0</v>
+      </c>
+      <c r="U115">
+        <v>0</v>
+      </c>
+      <c r="V115">
+        <v>0</v>
+      </c>
+      <c r="W115">
+        <v>11616</v>
+      </c>
+      <c r="X115" t="s">
+        <v>530</v>
+      </c>
+      <c r="Y115">
+        <v>5</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>700</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>698</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="G116">
+        <v>140</v>
+      </c>
+      <c r="H116" t="s">
+        <v>141</v>
+      </c>
+      <c r="I116">
+        <v>0.69</v>
+      </c>
+      <c r="J116">
+        <v>-7.02</v>
+      </c>
+      <c r="N116">
+        <v>2</v>
+      </c>
+      <c r="O116">
+        <v>0</v>
+      </c>
+      <c r="P116">
+        <v>0</v>
+      </c>
+      <c r="Q116">
+        <v>0</v>
+      </c>
+      <c r="R116">
+        <v>0</v>
+      </c>
+      <c r="S116">
+        <v>0</v>
+      </c>
+      <c r="T116">
+        <v>0</v>
+      </c>
+      <c r="U116">
+        <v>0</v>
+      </c>
+      <c r="V116">
+        <v>0</v>
+      </c>
+      <c r="W116" t="s">
+        <v>697</v>
+      </c>
+      <c r="X116" t="s">
+        <v>703</v>
+      </c>
+      <c r="Y116">
+        <v>5</v>
+      </c>
+      <c r="Z116" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="C122" s="17" t="s">
+        <v>684</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="E122" s="13" t="s">
+        <v>685</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G122">
+        <v>50</v>
+      </c>
+      <c r="H122" t="s">
+        <v>691</v>
+      </c>
+      <c r="N122">
+        <v>2</v>
+      </c>
+      <c r="O122">
+        <v>0</v>
+      </c>
+      <c r="P122">
+        <v>0</v>
+      </c>
+      <c r="Q122">
+        <v>0</v>
+      </c>
+      <c r="R122">
+        <v>0</v>
+      </c>
+      <c r="S122">
+        <v>0</v>
+      </c>
+      <c r="T122">
+        <v>0</v>
+      </c>
+      <c r="U122">
+        <v>0</v>
+      </c>
+      <c r="V122">
+        <v>0</v>
+      </c>
+      <c r="W122">
+        <v>11616</v>
+      </c>
+      <c r="X122" t="s">
+        <v>616</v>
+      </c>
+      <c r="Y122" t="s">
+        <v>552</v>
+      </c>
+      <c r="Z122" t="s">
+        <v>692</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A16:X33">
-    <cfRule type="expression" dxfId="121" priority="122">
+    <cfRule type="expression" dxfId="380" priority="143">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="125">
+    <cfRule type="expression" dxfId="379" priority="146">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="119" priority="121">
+    <cfRule type="expression" dxfId="378" priority="142">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="124">
+    <cfRule type="expression" dxfId="377" priority="145">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="117" priority="123">
+    <cfRule type="expression" dxfId="376" priority="144">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="116" priority="120">
+    <cfRule type="expression" dxfId="375" priority="141">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="expression" dxfId="115" priority="119">
+    <cfRule type="expression" dxfId="374" priority="140">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="114" priority="118">
+    <cfRule type="expression" dxfId="373" priority="139">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="113" priority="115">
+    <cfRule type="expression" dxfId="372" priority="136">
       <formula>$N73=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="117">
+    <cfRule type="expression" dxfId="371" priority="138">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="111" priority="116">
+    <cfRule type="expression" dxfId="370" priority="137">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="110" priority="112">
+    <cfRule type="expression" dxfId="369" priority="133">
       <formula>$N74=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="114">
+    <cfRule type="expression" dxfId="368" priority="135">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="108" priority="113">
+    <cfRule type="expression" dxfId="367" priority="134">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="107" priority="109">
+    <cfRule type="expression" dxfId="366" priority="130">
       <formula>$N75=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="111">
+    <cfRule type="expression" dxfId="365" priority="132">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="105" priority="110">
+    <cfRule type="expression" dxfId="364" priority="131">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="104" priority="106">
+    <cfRule type="expression" dxfId="363" priority="127">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="108">
+    <cfRule type="expression" dxfId="362" priority="129">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="102" priority="107">
+    <cfRule type="expression" dxfId="361" priority="128">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="101" priority="103">
+    <cfRule type="expression" dxfId="360" priority="124">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="105">
+    <cfRule type="expression" dxfId="359" priority="126">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="99" priority="104">
+    <cfRule type="expression" dxfId="358" priority="125">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="98" priority="100">
+    <cfRule type="expression" dxfId="357" priority="121">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="102">
+    <cfRule type="expression" dxfId="356" priority="123">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="96" priority="101">
+    <cfRule type="expression" dxfId="355" priority="122">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="95" priority="97">
+    <cfRule type="expression" dxfId="354" priority="118">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="99">
+    <cfRule type="expression" dxfId="353" priority="120">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="93" priority="98">
+    <cfRule type="expression" dxfId="352" priority="119">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="92" priority="94">
+    <cfRule type="expression" dxfId="351" priority="115">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="96">
+    <cfRule type="expression" dxfId="350" priority="117">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="90" priority="95">
+    <cfRule type="expression" dxfId="349" priority="116">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="89" priority="91">
+    <cfRule type="expression" dxfId="348" priority="112">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="93">
+    <cfRule type="expression" dxfId="347" priority="114">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="87" priority="92">
+    <cfRule type="expression" dxfId="346" priority="113">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="86" priority="88">
+    <cfRule type="expression" dxfId="345" priority="109">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="90">
+    <cfRule type="expression" dxfId="344" priority="111">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="84" priority="89">
+    <cfRule type="expression" dxfId="343" priority="110">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="83" priority="85">
+    <cfRule type="expression" dxfId="342" priority="106">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="87">
+    <cfRule type="expression" dxfId="341" priority="108">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="81" priority="86">
+    <cfRule type="expression" dxfId="340" priority="107">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y83:Y96">
-    <cfRule type="expression" dxfId="80" priority="82">
+    <cfRule type="expression" dxfId="339" priority="103">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="84">
+    <cfRule type="expression" dxfId="338" priority="105">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y83:Y96">
-    <cfRule type="expression" dxfId="78" priority="83">
+    <cfRule type="expression" dxfId="337" priority="104">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="77" priority="79">
+    <cfRule type="expression" dxfId="336" priority="100">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="81">
+    <cfRule type="expression" dxfId="335" priority="102">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="75" priority="80">
+    <cfRule type="expression" dxfId="334" priority="101">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="74" priority="76">
+    <cfRule type="expression" dxfId="333" priority="97">
       <formula>$N84=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="78">
+    <cfRule type="expression" dxfId="332" priority="99">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="72" priority="77">
+    <cfRule type="expression" dxfId="331" priority="98">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="71" priority="73">
+    <cfRule type="expression" dxfId="330" priority="94">
       <formula>$N85=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="75">
+    <cfRule type="expression" dxfId="329" priority="96">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="69" priority="74">
+    <cfRule type="expression" dxfId="328" priority="95">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="68" priority="70">
+    <cfRule type="expression" dxfId="327" priority="91">
       <formula>$N86=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="72">
+    <cfRule type="expression" dxfId="326" priority="93">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="66" priority="71">
+    <cfRule type="expression" dxfId="325" priority="92">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="65" priority="67">
+    <cfRule type="expression" dxfId="324" priority="88">
       <formula>$N87=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="69">
+    <cfRule type="expression" dxfId="323" priority="90">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="63" priority="68">
+    <cfRule type="expression" dxfId="322" priority="89">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="62" priority="64">
+    <cfRule type="expression" dxfId="321" priority="85">
       <formula>$N88=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="66">
+    <cfRule type="expression" dxfId="320" priority="87">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="60" priority="65">
+    <cfRule type="expression" dxfId="319" priority="86">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="59" priority="61">
+    <cfRule type="expression" dxfId="318" priority="82">
       <formula>$N89=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="63">
+    <cfRule type="expression" dxfId="317" priority="84">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="57" priority="62">
+    <cfRule type="expression" dxfId="316" priority="83">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="56" priority="58">
+    <cfRule type="expression" dxfId="315" priority="79">
       <formula>$N90=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="60">
+    <cfRule type="expression" dxfId="314" priority="81">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="54" priority="59">
+    <cfRule type="expression" dxfId="313" priority="80">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91:V91">
-    <cfRule type="expression" dxfId="53" priority="55">
+    <cfRule type="expression" dxfId="312" priority="76">
       <formula>$N91=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="57">
+    <cfRule type="expression" dxfId="311" priority="78">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91:V91">
-    <cfRule type="expression" dxfId="51" priority="56">
+    <cfRule type="expression" dxfId="310" priority="77">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92:W92">
-    <cfRule type="expression" dxfId="50" priority="52">
+    <cfRule type="expression" dxfId="309" priority="73">
       <formula>$N92=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="54">
+    <cfRule type="expression" dxfId="308" priority="75">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92:W92">
-    <cfRule type="expression" dxfId="48" priority="53">
+    <cfRule type="expression" dxfId="307" priority="74">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93:V93">
-    <cfRule type="expression" dxfId="47" priority="49">
+    <cfRule type="expression" dxfId="306" priority="70">
       <formula>$N93=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="51">
+    <cfRule type="expression" dxfId="305" priority="72">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93:V93">
-    <cfRule type="expression" dxfId="45" priority="50">
+    <cfRule type="expression" dxfId="304" priority="71">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="44" priority="46">
+    <cfRule type="expression" dxfId="303" priority="67">
       <formula>$N94=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="48">
+    <cfRule type="expression" dxfId="302" priority="69">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="42" priority="47">
+    <cfRule type="expression" dxfId="301" priority="68">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:W95">
-    <cfRule type="expression" dxfId="41" priority="43">
+    <cfRule type="expression" dxfId="300" priority="64">
       <formula>$N95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="45">
+    <cfRule type="expression" dxfId="299" priority="66">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:W95">
-    <cfRule type="expression" dxfId="39" priority="44">
+    <cfRule type="expression" dxfId="298" priority="65">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O96:V96">
-    <cfRule type="expression" dxfId="38" priority="37">
+    <cfRule type="expression" dxfId="297" priority="58">
       <formula>$N96=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="296" priority="60">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O96:V96">
-    <cfRule type="expression" dxfId="36" priority="38">
+    <cfRule type="expression" dxfId="295" priority="59">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y112">
-    <cfRule type="expression" dxfId="23" priority="22">
+  <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y116">
+    <cfRule type="expression" dxfId="294" priority="43">
       <formula>$N105=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="24">
+    <cfRule type="expression" dxfId="293" priority="45">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y112">
-    <cfRule type="expression" dxfId="21" priority="23">
+  <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y116">
+    <cfRule type="expression" dxfId="292" priority="44">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="291" priority="40">
       <formula>$N106=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
+    <cfRule type="expression" dxfId="290" priority="42">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="289" priority="41">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="288" priority="37">
       <formula>$N107=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="287" priority="39">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="286" priority="38">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="285" priority="34">
       <formula>$N108=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="284" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="283" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="282" priority="31">
       <formula>$N109=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="281" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="280" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="279" priority="28">
       <formula>$N110=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="278" priority="30">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="277" priority="29">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
+    <cfRule type="expression" dxfId="276" priority="25">
+      <formula>$N111=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="275" priority="27">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O111:V111">
+    <cfRule type="expression" dxfId="274" priority="26">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O112:V112">
+    <cfRule type="expression" dxfId="273" priority="22">
+      <formula>$N112=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="272" priority="24">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O112:V112">
+    <cfRule type="expression" dxfId="271" priority="23">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O113:V113">
+    <cfRule type="expression" dxfId="270" priority="19">
+      <formula>$N113=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="269" priority="21">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O113:V113">
+    <cfRule type="expression" dxfId="268" priority="20">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O114:V114">
+    <cfRule type="expression" dxfId="267" priority="16">
+      <formula>$N114=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="266" priority="18">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O114:V114">
+    <cfRule type="expression" dxfId="265" priority="17">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W122">
+    <cfRule type="expression" dxfId="261" priority="10">
+      <formula>$N122=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="260" priority="12">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W122">
+    <cfRule type="expression" dxfId="259" priority="11">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O122:V122">
+    <cfRule type="expression" dxfId="258" priority="7">
+      <formula>$N122=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="257" priority="9">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O122:V122">
+    <cfRule type="expression" dxfId="256" priority="8">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O115:V115">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N111=0</formula>
+      <formula>$N115=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O111:V111">
+  <conditionalFormatting sqref="O115:V115">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O112:V112">
+  <conditionalFormatting sqref="O116:V116">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N112=0</formula>
+      <formula>$N116=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O112:V112">
+  <conditionalFormatting sqref="O116:V116">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C112" r:id="rId1" display="https://cds.unistra.fr/cgi-bin/Dic-Simbad?%5bSCH2006b%5d" xr:uid="{9DD3F2B4-9683-7B49-8C86-4938A87017D6}"/>
+    <hyperlink ref="C122" r:id="rId2" display="https://cds.unistra.fr/cgi-bin/Dic-Simbad?CD-29" xr:uid="{0D00C683-1158-7344-B7D7-93941A710365}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>